<commit_message>
WorldMap implemented, added "Map" button
</commit_message>
<xml_diff>
--- a/Planning/OverworldMap.xlsx
+++ b/Planning/OverworldMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Repos\ZeldasAdventureRemastered\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812E2FFA-446D-4049-AF5B-6915EFB27190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF96B757-FB13-4F2C-8560-CB4911D58863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{2A32EC26-D8CF-452B-B3E7-5B8DBE295FDC}"/>
+    <workbookView xWindow="44025" yWindow="1170" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{2A32EC26-D8CF-452B-B3E7-5B8DBE295FDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Music" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="161">
   <si>
     <t>Shrine_Earth_01</t>
   </si>
@@ -504,9 +504,6 @@
   </si>
   <si>
     <t>163 181</t>
-  </si>
-  <si>
-    <t>292 293</t>
   </si>
   <si>
     <t>227 228</t>
@@ -833,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1017,23 +1014,26 @@
     <xf numFmtId="0" fontId="2" fillId="29" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6301,9 +6301,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9537CFE-57F2-4F28-80FA-85CCA398DEFA}">
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q24" sqref="Q24"/>
+      <selection pane="topRight" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8053,7 +8053,7 @@
       <c r="H33" s="43">
         <v>292</v>
       </c>
-      <c r="I33" s="52">
+      <c r="I33" s="43">
         <v>293</v>
       </c>
       <c r="J33" s="46"/>
@@ -8349,9 +8349,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C60D82-0D39-41C8-82A6-6A9D39131FF7}">
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O12" sqref="O12"/>
+      <selection pane="topRight" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8369,1697 +8369,1744 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="45" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63">
+      <c r="A1" s="64"/>
+      <c r="B1" s="64">
         <v>0</v>
       </c>
-      <c r="C1" s="63">
+      <c r="C1" s="64">
         <v>1</v>
       </c>
-      <c r="D1" s="63">
+      <c r="D1" s="64">
         <v>2</v>
       </c>
-      <c r="E1" s="63">
+      <c r="E1" s="64">
         <v>3</v>
       </c>
-      <c r="F1" s="63">
+      <c r="F1" s="64">
         <v>4</v>
       </c>
-      <c r="G1" s="63">
+      <c r="G1" s="64">
         <v>5</v>
       </c>
-      <c r="H1" s="63">
+      <c r="H1" s="64">
         <v>6</v>
       </c>
-      <c r="I1" s="63">
+      <c r="I1" s="64">
         <v>7</v>
       </c>
-      <c r="J1" s="63">
+      <c r="J1" s="64">
         <v>8</v>
       </c>
-      <c r="K1" s="63">
+      <c r="K1" s="64">
         <v>9</v>
       </c>
-      <c r="L1" s="63">
+      <c r="L1" s="64">
         <v>10</v>
       </c>
-      <c r="M1" s="63">
+      <c r="M1" s="64">
         <v>11</v>
       </c>
-      <c r="N1" s="63">
+      <c r="N1" s="64">
         <v>12</v>
       </c>
-      <c r="O1" s="63">
+      <c r="O1" s="64">
         <v>13</v>
       </c>
-      <c r="P1" s="63">
+      <c r="P1" s="64">
         <v>14</v>
       </c>
-      <c r="Q1" s="63">
+      <c r="Q1" s="64">
         <v>15</v>
       </c>
-      <c r="R1" s="63">
+      <c r="R1" s="64">
         <v>16</v>
       </c>
-      <c r="S1" s="63">
+      <c r="S1" s="64">
         <v>17</v>
       </c>
-      <c r="T1" s="63">
+      <c r="T1" s="64">
         <v>18</v>
       </c>
-      <c r="U1" s="63">
+      <c r="U1" s="64">
         <v>19</v>
       </c>
-      <c r="V1" s="63">
+      <c r="V1" s="64">
         <v>20</v>
       </c>
-      <c r="W1" s="63">
+      <c r="W1" s="64">
         <v>21</v>
       </c>
-      <c r="X1" s="63">
+      <c r="X1" s="64">
         <v>22</v>
       </c>
-      <c r="Y1" s="63">
+      <c r="Y1" s="64">
         <v>23</v>
       </c>
-      <c r="Z1" s="63">
+      <c r="Z1" s="64">
         <v>24</v>
       </c>
-      <c r="AA1" s="63">
+      <c r="AA1" s="64">
         <v>25</v>
       </c>
-      <c r="AB1" s="63">
+      <c r="AB1" s="64">
         <v>26</v>
       </c>
-      <c r="AC1" s="63">
+      <c r="AC1" s="64">
         <v>27</v>
       </c>
-      <c r="AD1" s="63">
+      <c r="AD1" s="64">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63">
+      <c r="A2" s="64">
         <v>0</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="65">
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="66">
         <v>0</v>
       </c>
-      <c r="AB2" s="64"/>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64"/>
+      <c r="AB2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
     </row>
     <row r="3" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63">
+      <c r="A3" s="64">
         <v>1</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="65">
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
+      <c r="X3" s="65"/>
+      <c r="Y3" s="65"/>
+      <c r="Z3" s="65"/>
+      <c r="AA3" s="66">
         <v>1</v>
       </c>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
+      <c r="AB3" s="65"/>
+      <c r="AC3" s="65"/>
+      <c r="AD3" s="65"/>
     </row>
     <row r="4" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="63">
+      <c r="A4" s="64">
         <v>2</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
-      <c r="X4" s="64"/>
-      <c r="Y4" s="64"/>
-      <c r="Z4" s="65">
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
+      <c r="U4" s="65"/>
+      <c r="V4" s="65"/>
+      <c r="W4" s="65"/>
+      <c r="X4" s="65"/>
+      <c r="Y4" s="65"/>
+      <c r="Z4" s="66">
         <v>2</v>
       </c>
-      <c r="AA4" s="65">
+      <c r="AA4" s="66">
         <v>3</v>
       </c>
-      <c r="AB4" s="64"/>
-      <c r="AC4" s="64"/>
-      <c r="AD4" s="64"/>
+      <c r="AB4" s="65"/>
+      <c r="AC4" s="65"/>
+      <c r="AD4" s="65"/>
     </row>
     <row r="5" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="63">
+      <c r="A5" s="64">
         <v>3</v>
       </c>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="64"/>
-      <c r="J5" s="64"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="64"/>
-      <c r="N5" s="64"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="64"/>
-      <c r="Q5" s="64"/>
-      <c r="R5" s="64"/>
-      <c r="S5" s="64"/>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64"/>
-      <c r="W5" s="64"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="64"/>
-      <c r="Z5" s="65">
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="65"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="65"/>
+      <c r="Z5" s="66">
         <v>4</v>
       </c>
-      <c r="AA5" s="65">
+      <c r="AA5" s="66">
         <v>5</v>
       </c>
-      <c r="AB5" s="64"/>
-      <c r="AC5" s="64"/>
-      <c r="AD5" s="64"/>
+      <c r="AB5" s="65"/>
+      <c r="AC5" s="65"/>
+      <c r="AD5" s="65"/>
     </row>
     <row r="6" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="63">
+      <c r="A6" s="64">
         <v>4</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="64"/>
-      <c r="P6" s="64"/>
-      <c r="Q6" s="64"/>
-      <c r="R6" s="64"/>
-      <c r="S6" s="65">
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="66">
         <v>6</v>
       </c>
-      <c r="T6" s="65">
+      <c r="T6" s="66">
         <v>7</v>
       </c>
-      <c r="U6" s="64"/>
-      <c r="W6" s="65">
+      <c r="U6" s="65"/>
+      <c r="V6" s="65"/>
+      <c r="W6" s="66">
         <v>9</v>
       </c>
-      <c r="X6" s="65">
+      <c r="X6" s="66">
         <v>10</v>
       </c>
-      <c r="Y6" s="65">
+      <c r="Y6" s="66">
         <v>11</v>
       </c>
-      <c r="Z6" s="65">
+      <c r="Z6" s="66">
         <v>12</v>
       </c>
-      <c r="AA6" s="65">
+      <c r="AA6" s="66">
         <v>13</v>
       </c>
-      <c r="AB6" s="64"/>
-      <c r="AC6" s="64"/>
-      <c r="AD6" s="64"/>
+      <c r="AB6" s="65"/>
+      <c r="AC6" s="65"/>
+      <c r="AD6" s="65"/>
     </row>
     <row r="7" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="63">
+      <c r="A7" s="64">
         <v>5</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="64"/>
-      <c r="S7" s="65">
+      <c r="B7" s="65"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65"/>
+      <c r="R7" s="65"/>
+      <c r="S7" s="66">
         <v>14</v>
       </c>
-      <c r="T7" s="65">
+      <c r="T7" s="66">
         <v>15</v>
       </c>
-      <c r="U7" s="66" t="s">
+      <c r="U7" s="67" t="s">
+        <v>160</v>
+      </c>
+      <c r="V7" s="65"/>
+      <c r="W7" s="66">
+        <v>17</v>
+      </c>
+      <c r="X7" s="66">
+        <v>18</v>
+      </c>
+      <c r="Y7" s="66">
+        <v>19</v>
+      </c>
+      <c r="Z7" s="66">
+        <v>20</v>
+      </c>
+      <c r="AA7" s="66">
+        <v>21</v>
+      </c>
+      <c r="AB7" s="65"/>
+      <c r="AC7" s="65"/>
+      <c r="AD7" s="65"/>
+    </row>
+    <row r="8" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="64">
+        <v>6</v>
+      </c>
+      <c r="B8" s="66">
+        <v>22</v>
+      </c>
+      <c r="C8" s="66">
+        <v>23</v>
+      </c>
+      <c r="D8" s="66">
+        <v>24</v>
+      </c>
+      <c r="E8" s="66">
+        <v>25</v>
+      </c>
+      <c r="F8" s="66">
+        <v>26</v>
+      </c>
+      <c r="G8" s="66">
+        <v>27</v>
+      </c>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="65"/>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+      <c r="N8" s="65"/>
+      <c r="O8" s="65"/>
+      <c r="P8" s="65"/>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="65"/>
+      <c r="S8" s="66">
+        <v>29</v>
+      </c>
+      <c r="T8" s="66">
+        <v>30</v>
+      </c>
+      <c r="U8" s="65"/>
+      <c r="V8" s="65"/>
+      <c r="W8" s="66">
+        <v>31</v>
+      </c>
+      <c r="X8" s="66">
+        <v>32</v>
+      </c>
+      <c r="Y8" s="66">
+        <v>33</v>
+      </c>
+      <c r="Z8" s="65"/>
+      <c r="AA8" s="65"/>
+      <c r="AB8" s="65"/>
+      <c r="AC8" s="65"/>
+      <c r="AD8" s="65"/>
+    </row>
+    <row r="9" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="64">
+        <v>7</v>
+      </c>
+      <c r="B9" s="66">
+        <v>34</v>
+      </c>
+      <c r="C9" s="66">
+        <v>35</v>
+      </c>
+      <c r="D9" s="66">
+        <v>36</v>
+      </c>
+      <c r="E9" s="66">
+        <v>37</v>
+      </c>
+      <c r="F9" s="66">
+        <v>38</v>
+      </c>
+      <c r="G9" s="66">
+        <v>39</v>
+      </c>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="66">
+        <v>40</v>
+      </c>
+      <c r="N9" s="66">
+        <v>41</v>
+      </c>
+      <c r="O9" s="66">
+        <v>42</v>
+      </c>
+      <c r="P9" s="66">
+        <v>43</v>
+      </c>
+      <c r="Q9" s="66">
+        <v>44</v>
+      </c>
+      <c r="R9" s="66">
+        <v>45</v>
+      </c>
+      <c r="S9" s="66">
+        <v>46</v>
+      </c>
+      <c r="T9" s="66">
+        <v>47</v>
+      </c>
+      <c r="U9" s="66">
+        <v>48</v>
+      </c>
+      <c r="V9" s="65"/>
+      <c r="W9" s="66">
+        <v>49</v>
+      </c>
+      <c r="X9" s="66">
+        <v>50</v>
+      </c>
+      <c r="Y9" s="66">
+        <v>51</v>
+      </c>
+      <c r="Z9" s="65"/>
+      <c r="AA9" s="65"/>
+      <c r="AB9" s="65"/>
+      <c r="AC9" s="65"/>
+      <c r="AD9" s="65"/>
+    </row>
+    <row r="10" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="64">
+        <v>8</v>
+      </c>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="66">
+        <v>52</v>
+      </c>
+      <c r="G10" s="66">
+        <v>53</v>
+      </c>
+      <c r="H10" s="66">
+        <v>54</v>
+      </c>
+      <c r="I10" s="66">
+        <v>55</v>
+      </c>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="66">
+        <v>56</v>
+      </c>
+      <c r="N10" s="66">
+        <v>57</v>
+      </c>
+      <c r="O10" s="66">
+        <v>58</v>
+      </c>
+      <c r="P10" s="66">
+        <v>59</v>
+      </c>
+      <c r="Q10" s="66">
+        <v>60</v>
+      </c>
+      <c r="R10" s="66">
+        <v>61</v>
+      </c>
+      <c r="S10" s="66">
+        <v>62</v>
+      </c>
+      <c r="T10" s="65"/>
+      <c r="U10" s="65"/>
+      <c r="V10" s="65"/>
+      <c r="W10" s="66">
+        <v>63</v>
+      </c>
+      <c r="X10" s="66">
+        <v>64</v>
+      </c>
+      <c r="Y10" s="66">
+        <v>65</v>
+      </c>
+      <c r="Z10" s="65"/>
+      <c r="AA10" s="65"/>
+      <c r="AB10" s="65"/>
+      <c r="AC10" s="65"/>
+      <c r="AD10" s="65"/>
+    </row>
+    <row r="11" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="64">
+        <v>9</v>
+      </c>
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="66">
+        <v>66</v>
+      </c>
+      <c r="G11" s="66">
+        <v>67</v>
+      </c>
+      <c r="H11" s="66">
+        <v>68</v>
+      </c>
+      <c r="I11" s="66">
+        <v>69</v>
+      </c>
+      <c r="J11" s="66">
+        <v>70</v>
+      </c>
+      <c r="K11" s="66">
+        <v>71</v>
+      </c>
+      <c r="L11" s="66">
+        <v>72</v>
+      </c>
+      <c r="M11" s="66">
+        <v>73</v>
+      </c>
+      <c r="N11" s="66">
+        <v>74</v>
+      </c>
+      <c r="O11" s="66">
+        <v>75</v>
+      </c>
+      <c r="P11" s="66">
+        <v>76</v>
+      </c>
+      <c r="Q11" s="66">
+        <v>77</v>
+      </c>
+      <c r="R11" s="66">
+        <v>78</v>
+      </c>
+      <c r="S11" s="66">
+        <v>79</v>
+      </c>
+      <c r="T11" s="65"/>
+      <c r="U11" s="65"/>
+      <c r="V11" s="65"/>
+      <c r="W11" s="66">
+        <v>80</v>
+      </c>
+      <c r="X11" s="66">
+        <v>81</v>
+      </c>
+      <c r="Y11" s="66">
+        <v>82</v>
+      </c>
+      <c r="Z11" s="65"/>
+      <c r="AA11" s="65"/>
+      <c r="AB11" s="65"/>
+      <c r="AC11" s="65"/>
+      <c r="AD11" s="65"/>
+    </row>
+    <row r="12" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="64">
+        <v>10</v>
+      </c>
+      <c r="B12" s="65"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="66">
+        <v>83</v>
+      </c>
+      <c r="I12" s="66">
+        <v>84</v>
+      </c>
+      <c r="J12" s="66">
+        <v>85</v>
+      </c>
+      <c r="K12" s="66">
+        <v>86</v>
+      </c>
+      <c r="L12" s="66">
+        <v>87</v>
+      </c>
+      <c r="M12" s="66">
+        <v>88</v>
+      </c>
+      <c r="N12" s="66">
+        <v>89</v>
+      </c>
+      <c r="O12" s="67" t="s">
+        <v>155</v>
+      </c>
+      <c r="P12" s="67" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q12" s="66">
+        <v>92</v>
+      </c>
+      <c r="R12" s="65"/>
+      <c r="S12" s="65"/>
+      <c r="T12" s="65"/>
+      <c r="U12" s="65"/>
+      <c r="V12" s="65"/>
+      <c r="W12" s="66">
+        <v>94</v>
+      </c>
+      <c r="X12" s="66">
+        <v>95</v>
+      </c>
+      <c r="Y12" s="66">
+        <v>96</v>
+      </c>
+      <c r="Z12" s="65"/>
+      <c r="AA12" s="65"/>
+      <c r="AB12" s="65"/>
+      <c r="AC12" s="65"/>
+      <c r="AD12" s="65"/>
+    </row>
+    <row r="13" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="64">
+        <v>11</v>
+      </c>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="66">
+        <v>100</v>
+      </c>
+      <c r="M13" s="66">
+        <v>101</v>
+      </c>
+      <c r="N13" s="66">
+        <v>102</v>
+      </c>
+      <c r="O13" s="66">
+        <v>103</v>
+      </c>
+      <c r="P13" s="66">
+        <v>104</v>
+      </c>
+      <c r="Q13" s="66">
+        <v>105</v>
+      </c>
+      <c r="R13" s="65"/>
+      <c r="S13" s="65"/>
+      <c r="T13" s="65"/>
+      <c r="U13" s="65"/>
+      <c r="V13" s="65"/>
+      <c r="W13" s="66">
+        <v>106</v>
+      </c>
+      <c r="X13" s="66">
+        <v>107</v>
+      </c>
+      <c r="Y13" s="66">
+        <v>108</v>
+      </c>
+      <c r="Z13" s="65"/>
+      <c r="AA13" s="65"/>
+      <c r="AB13" s="65"/>
+      <c r="AC13" s="65"/>
+      <c r="AD13" s="65"/>
+    </row>
+    <row r="14" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="64">
+        <v>12</v>
+      </c>
+      <c r="B14" s="65"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="M14" s="67" t="s">
+        <v>153</v>
+      </c>
+      <c r="N14" s="66">
+        <v>112</v>
+      </c>
+      <c r="O14" s="66">
+        <v>113</v>
+      </c>
+      <c r="P14" s="66">
+        <v>114</v>
+      </c>
+      <c r="Q14" s="66">
+        <v>115</v>
+      </c>
+      <c r="R14" s="66">
+        <v>116</v>
+      </c>
+      <c r="S14" s="65"/>
+      <c r="T14" s="65"/>
+      <c r="U14" s="65"/>
+      <c r="V14" s="65"/>
+      <c r="W14" s="65"/>
+      <c r="X14" s="66">
+        <v>117</v>
+      </c>
+      <c r="Y14" s="65"/>
+      <c r="Z14" s="65"/>
+      <c r="AA14" s="66">
+        <v>118</v>
+      </c>
+      <c r="AB14" s="65"/>
+      <c r="AC14" s="65"/>
+      <c r="AD14" s="65"/>
+    </row>
+    <row r="15" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="64">
+        <v>13</v>
+      </c>
+      <c r="B15" s="65"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="K15" s="65"/>
+      <c r="L15" s="66">
+        <v>119</v>
+      </c>
+      <c r="M15" s="66">
+        <v>120</v>
+      </c>
+      <c r="N15" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="O15" s="66">
+        <v>122</v>
+      </c>
+      <c r="P15" s="66">
+        <v>123</v>
+      </c>
+      <c r="Q15" s="66">
+        <v>124</v>
+      </c>
+      <c r="R15" s="66">
+        <v>125</v>
+      </c>
+      <c r="S15" s="65"/>
+      <c r="T15" s="65"/>
+      <c r="U15" s="66">
+        <v>126</v>
+      </c>
+      <c r="V15" s="66">
+        <v>127</v>
+      </c>
+      <c r="W15" s="66">
+        <v>128</v>
+      </c>
+      <c r="X15" s="66">
+        <v>129</v>
+      </c>
+      <c r="Y15" s="66">
+        <v>130</v>
+      </c>
+      <c r="Z15" s="66">
+        <v>131</v>
+      </c>
+      <c r="AA15" s="66">
+        <v>132</v>
+      </c>
+      <c r="AB15" s="65"/>
+      <c r="AC15" s="65"/>
+      <c r="AD15" s="65"/>
+    </row>
+    <row r="16" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="64">
+        <v>14</v>
+      </c>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="65"/>
+      <c r="K16" s="66">
+        <v>133</v>
+      </c>
+      <c r="L16" s="66">
+        <v>134</v>
+      </c>
+      <c r="M16" s="66">
+        <v>135</v>
+      </c>
+      <c r="N16" s="66">
+        <v>136</v>
+      </c>
+      <c r="O16" s="66">
+        <v>137</v>
+      </c>
+      <c r="P16" s="66">
+        <v>138</v>
+      </c>
+      <c r="Q16" s="66">
+        <v>139</v>
+      </c>
+      <c r="R16" s="66">
+        <v>140</v>
+      </c>
+      <c r="S16" s="66">
+        <v>141</v>
+      </c>
+      <c r="T16" s="66">
+        <v>142</v>
+      </c>
+      <c r="U16" s="66">
+        <v>143</v>
+      </c>
+      <c r="V16" s="66">
+        <v>144</v>
+      </c>
+      <c r="W16" s="66">
+        <v>145</v>
+      </c>
+      <c r="X16" s="66">
+        <v>146</v>
+      </c>
+      <c r="Y16" s="66">
+        <v>147</v>
+      </c>
+      <c r="Z16" s="66">
+        <v>148</v>
+      </c>
+      <c r="AA16" s="66">
+        <v>149</v>
+      </c>
+      <c r="AB16" s="66">
+        <v>150</v>
+      </c>
+      <c r="AC16" s="65"/>
+      <c r="AD16" s="65"/>
+    </row>
+    <row r="17" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="64">
+        <v>15</v>
+      </c>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="65"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
+      <c r="K17" s="66">
+        <v>151</v>
+      </c>
+      <c r="L17" s="66">
+        <v>152</v>
+      </c>
+      <c r="M17" s="66">
+        <v>153</v>
+      </c>
+      <c r="N17" s="66">
+        <v>154</v>
+      </c>
+      <c r="O17" s="66">
+        <v>155</v>
+      </c>
+      <c r="P17" s="66">
+        <v>156</v>
+      </c>
+      <c r="Q17" s="66">
+        <v>157</v>
+      </c>
+      <c r="R17" s="66">
+        <v>158</v>
+      </c>
+      <c r="S17" s="66">
+        <v>159</v>
+      </c>
+      <c r="T17" s="66">
+        <v>160</v>
+      </c>
+      <c r="U17" s="66">
         <v>161</v>
       </c>
-      <c r="V7" s="64"/>
-      <c r="W7" s="65">
+      <c r="V17" s="66">
+        <v>162</v>
+      </c>
+      <c r="W17" s="67" t="s">
+        <v>157</v>
+      </c>
+      <c r="X17" s="66">
+        <v>164</v>
+      </c>
+      <c r="Y17" s="66">
+        <v>165</v>
+      </c>
+      <c r="Z17" s="66">
+        <v>166</v>
+      </c>
+      <c r="AA17" s="66">
+        <v>167</v>
+      </c>
+      <c r="AB17" s="66">
+        <v>168</v>
+      </c>
+      <c r="AC17" s="65"/>
+      <c r="AD17" s="65"/>
+    </row>
+    <row r="18" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="64">
+        <v>16</v>
+      </c>
+      <c r="B18" s="68"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="66">
+        <v>169</v>
+      </c>
+      <c r="L18" s="66">
+        <v>170</v>
+      </c>
+      <c r="M18" s="66">
+        <v>171</v>
+      </c>
+      <c r="N18" s="66">
+        <v>172</v>
+      </c>
+      <c r="O18" s="66">
+        <v>173</v>
+      </c>
+      <c r="P18" s="66">
+        <v>174</v>
+      </c>
+      <c r="Q18" s="65"/>
+      <c r="R18" s="66">
+        <v>175</v>
+      </c>
+      <c r="S18" s="66">
+        <v>176</v>
+      </c>
+      <c r="T18" s="66">
+        <v>177</v>
+      </c>
+      <c r="U18" s="66">
+        <v>178</v>
+      </c>
+      <c r="V18" s="66">
+        <v>179</v>
+      </c>
+      <c r="W18" s="66">
+        <v>180</v>
+      </c>
+      <c r="X18" s="65"/>
+      <c r="Y18" s="65"/>
+      <c r="Z18" s="66">
+        <v>182</v>
+      </c>
+      <c r="AA18" s="66">
+        <v>183</v>
+      </c>
+      <c r="AB18" s="66">
+        <v>184</v>
+      </c>
+      <c r="AC18" s="66">
+        <v>185</v>
+      </c>
+      <c r="AD18" s="66">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="64">
         <v>17</v>
       </c>
-      <c r="X7" s="65">
+      <c r="B19" s="65"/>
+      <c r="C19" s="65"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
+      <c r="K19" s="65"/>
+      <c r="L19" s="66">
+        <v>187</v>
+      </c>
+      <c r="M19" s="66">
+        <v>188</v>
+      </c>
+      <c r="N19" s="66">
+        <v>189</v>
+      </c>
+      <c r="O19" s="66">
+        <v>190</v>
+      </c>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="65"/>
+      <c r="R19" s="66">
+        <v>191</v>
+      </c>
+      <c r="S19" s="66">
+        <v>192</v>
+      </c>
+      <c r="T19" s="66">
+        <v>193</v>
+      </c>
+      <c r="U19" s="66">
+        <v>194</v>
+      </c>
+      <c r="V19" s="66">
+        <v>195</v>
+      </c>
+      <c r="W19" s="66">
+        <v>196</v>
+      </c>
+      <c r="X19" s="65"/>
+      <c r="Y19" s="65"/>
+      <c r="Z19" s="65"/>
+      <c r="AA19" s="65"/>
+      <c r="AB19" s="65"/>
+      <c r="AC19" s="65"/>
+      <c r="AD19" s="66">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="64">
         <v>18</v>
       </c>
-      <c r="Y7" s="65">
+      <c r="B20" s="65"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="66">
+        <v>198</v>
+      </c>
+      <c r="M20" s="66">
+        <v>199</v>
+      </c>
+      <c r="N20" s="66">
+        <v>200</v>
+      </c>
+      <c r="O20" s="65"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="69"/>
+      <c r="R20" s="66">
+        <v>202</v>
+      </c>
+      <c r="S20" s="66">
+        <v>203</v>
+      </c>
+      <c r="T20" s="66">
+        <v>204</v>
+      </c>
+      <c r="U20" s="66">
+        <v>205</v>
+      </c>
+      <c r="V20" s="66">
+        <v>206</v>
+      </c>
+      <c r="W20" s="66">
+        <v>207</v>
+      </c>
+      <c r="X20" s="65"/>
+      <c r="Y20" s="65"/>
+      <c r="Z20" s="65"/>
+      <c r="AA20" s="65"/>
+      <c r="AB20" s="65"/>
+      <c r="AC20" s="65"/>
+      <c r="AD20" s="65"/>
+    </row>
+    <row r="21" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="64">
         <v>19</v>
       </c>
-      <c r="Z7" s="65">
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="66">
+        <v>208</v>
+      </c>
+      <c r="G21" s="66">
+        <v>209</v>
+      </c>
+      <c r="H21" s="66">
+        <v>210</v>
+      </c>
+      <c r="I21" s="66">
+        <v>211</v>
+      </c>
+      <c r="J21" s="66">
+        <v>212</v>
+      </c>
+      <c r="K21" s="66">
+        <v>213</v>
+      </c>
+      <c r="L21" s="66">
+        <v>214</v>
+      </c>
+      <c r="M21" s="65"/>
+      <c r="N21" s="65"/>
+      <c r="O21" s="65"/>
+      <c r="P21" s="65"/>
+      <c r="Q21" s="67" t="s">
+        <v>156</v>
+      </c>
+      <c r="R21" s="66">
+        <v>216</v>
+      </c>
+      <c r="S21" s="66">
+        <v>217</v>
+      </c>
+      <c r="T21" s="66">
+        <v>218</v>
+      </c>
+      <c r="U21" s="66">
+        <v>219</v>
+      </c>
+      <c r="V21" s="66">
+        <v>220</v>
+      </c>
+      <c r="W21" s="66">
+        <v>221</v>
+      </c>
+      <c r="X21" s="65"/>
+      <c r="Y21" s="65"/>
+      <c r="Z21" s="65"/>
+      <c r="AA21" s="65"/>
+      <c r="AB21" s="65"/>
+      <c r="AC21" s="65"/>
+      <c r="AD21" s="65"/>
+    </row>
+    <row r="22" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="64">
         <v>20</v>
       </c>
-      <c r="AA7" s="65">
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="66">
+        <v>222</v>
+      </c>
+      <c r="G22" s="66">
+        <v>223</v>
+      </c>
+      <c r="H22" s="66">
+        <v>224</v>
+      </c>
+      <c r="I22" s="66">
+        <v>225</v>
+      </c>
+      <c r="J22" s="66">
+        <v>226</v>
+      </c>
+      <c r="K22" s="67" t="s">
+        <v>158</v>
+      </c>
+      <c r="L22" s="65"/>
+      <c r="M22" s="65"/>
+      <c r="N22" s="65"/>
+      <c r="O22" s="65"/>
+      <c r="P22" s="65"/>
+      <c r="Q22" s="66">
+        <v>229</v>
+      </c>
+      <c r="R22" s="65"/>
+      <c r="S22" s="65"/>
+      <c r="T22" s="65"/>
+      <c r="U22" s="65"/>
+      <c r="V22" s="65"/>
+      <c r="W22" s="65"/>
+      <c r="X22" s="65"/>
+      <c r="Y22" s="65"/>
+      <c r="Z22" s="65"/>
+      <c r="AA22" s="65"/>
+      <c r="AB22" s="65"/>
+      <c r="AC22" s="65"/>
+      <c r="AD22" s="65"/>
+    </row>
+    <row r="23" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="64">
         <v>21</v>
       </c>
-      <c r="AB7" s="64"/>
-      <c r="AC7" s="64"/>
-      <c r="AD7" s="64"/>
-    </row>
-    <row r="8" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="63">
-        <v>6</v>
-      </c>
-      <c r="B8" s="65">
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="66">
+        <v>230</v>
+      </c>
+      <c r="G23" s="66">
+        <v>231</v>
+      </c>
+      <c r="H23" s="66">
+        <v>232</v>
+      </c>
+      <c r="I23" s="66">
+        <v>233</v>
+      </c>
+      <c r="J23" s="66">
+        <v>234</v>
+      </c>
+      <c r="K23" s="67" t="s">
+        <v>151</v>
+      </c>
+      <c r="L23" s="68"/>
+      <c r="M23" s="65"/>
+      <c r="N23" s="65"/>
+      <c r="O23" s="65"/>
+      <c r="P23" s="66">
+        <v>237</v>
+      </c>
+      <c r="Q23" s="66">
+        <v>238</v>
+      </c>
+      <c r="R23" s="65"/>
+      <c r="S23" s="65"/>
+      <c r="T23" s="65"/>
+      <c r="U23" s="65"/>
+      <c r="V23" s="65"/>
+      <c r="W23" s="65"/>
+      <c r="X23" s="65"/>
+      <c r="Y23" s="65"/>
+      <c r="Z23" s="65"/>
+      <c r="AA23" s="65"/>
+      <c r="AB23" s="65"/>
+      <c r="AC23" s="65"/>
+      <c r="AD23" s="65"/>
+    </row>
+    <row r="24" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="64">
         <v>22</v>
       </c>
-      <c r="C8" s="65">
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="66">
+        <v>239</v>
+      </c>
+      <c r="G24" s="66">
+        <v>240</v>
+      </c>
+      <c r="H24" s="66">
+        <v>241</v>
+      </c>
+      <c r="I24" s="66">
+        <v>242</v>
+      </c>
+      <c r="J24" s="66">
+        <v>243</v>
+      </c>
+      <c r="K24" s="66">
+        <v>244</v>
+      </c>
+      <c r="L24" s="65"/>
+      <c r="M24" s="65"/>
+      <c r="N24" s="65"/>
+      <c r="O24" s="65"/>
+      <c r="P24" s="66">
+        <v>245</v>
+      </c>
+      <c r="Q24" s="65"/>
+      <c r="R24" s="65"/>
+      <c r="S24" s="65"/>
+      <c r="T24" s="65"/>
+      <c r="U24" s="65"/>
+      <c r="V24" s="65"/>
+      <c r="W24" s="65"/>
+      <c r="X24" s="65"/>
+      <c r="Y24" s="65"/>
+      <c r="Z24" s="65"/>
+      <c r="AA24" s="65"/>
+      <c r="AB24" s="65"/>
+      <c r="AC24" s="65"/>
+      <c r="AD24" s="65"/>
+    </row>
+    <row r="25" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="64">
         <v>23</v>
       </c>
-      <c r="D8" s="65">
+      <c r="B25" s="65"/>
+      <c r="C25" s="65"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="66">
+        <v>246</v>
+      </c>
+      <c r="F25" s="66">
+        <v>247</v>
+      </c>
+      <c r="G25" s="66">
+        <v>248</v>
+      </c>
+      <c r="H25" s="66">
+        <v>249</v>
+      </c>
+      <c r="I25" s="66">
+        <v>250</v>
+      </c>
+      <c r="J25" s="66">
+        <v>251</v>
+      </c>
+      <c r="K25" s="66">
+        <v>252</v>
+      </c>
+      <c r="L25" s="65"/>
+      <c r="M25" s="65"/>
+      <c r="N25" s="65"/>
+      <c r="O25" s="65"/>
+      <c r="P25" s="66">
+        <v>254</v>
+      </c>
+      <c r="Q25" s="65"/>
+      <c r="R25" s="65"/>
+      <c r="S25" s="65"/>
+      <c r="T25" s="65"/>
+      <c r="U25" s="65"/>
+      <c r="V25" s="65"/>
+      <c r="W25" s="65"/>
+      <c r="X25" s="65"/>
+      <c r="Y25" s="65"/>
+      <c r="Z25" s="65"/>
+      <c r="AA25" s="65"/>
+      <c r="AB25" s="65"/>
+      <c r="AC25" s="65"/>
+      <c r="AD25" s="65"/>
+    </row>
+    <row r="26" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="64">
         <v>24</v>
       </c>
-      <c r="E8" s="65">
+      <c r="B26" s="65"/>
+      <c r="C26" s="65"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="66">
+        <v>255</v>
+      </c>
+      <c r="H26" s="66">
+        <v>256</v>
+      </c>
+      <c r="I26" s="66">
+        <v>257</v>
+      </c>
+      <c r="J26" s="66">
+        <v>258</v>
+      </c>
+      <c r="K26" s="66">
+        <v>259</v>
+      </c>
+      <c r="L26" s="65"/>
+      <c r="M26" s="65"/>
+      <c r="N26" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="O26" s="66">
+        <v>261</v>
+      </c>
+      <c r="P26" s="66">
+        <v>262</v>
+      </c>
+      <c r="Q26" s="65"/>
+      <c r="R26" s="65"/>
+      <c r="S26" s="65"/>
+      <c r="T26" s="65"/>
+      <c r="U26" s="65"/>
+      <c r="V26" s="65"/>
+      <c r="W26" s="65"/>
+      <c r="X26" s="65"/>
+      <c r="Y26" s="65"/>
+      <c r="Z26" s="65"/>
+      <c r="AA26" s="65"/>
+      <c r="AB26" s="65"/>
+      <c r="AC26" s="65"/>
+      <c r="AD26" s="65"/>
+    </row>
+    <row r="27" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="64">
         <v>25</v>
       </c>
-      <c r="F8" s="65">
+      <c r="B27" s="65"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="66">
+        <v>263</v>
+      </c>
+      <c r="H27" s="66">
+        <v>264</v>
+      </c>
+      <c r="I27" s="66">
+        <v>265</v>
+      </c>
+      <c r="J27" s="66">
+        <v>266</v>
+      </c>
+      <c r="K27" s="66">
+        <v>267</v>
+      </c>
+      <c r="L27" s="65"/>
+      <c r="M27" s="65"/>
+      <c r="N27" s="66">
+        <v>269</v>
+      </c>
+      <c r="O27" s="65"/>
+      <c r="P27" s="65"/>
+      <c r="Q27" s="65"/>
+      <c r="R27" s="65"/>
+      <c r="S27" s="65"/>
+      <c r="T27" s="65"/>
+      <c r="U27" s="65"/>
+      <c r="V27" s="65"/>
+      <c r="W27" s="65"/>
+      <c r="X27" s="65"/>
+      <c r="Y27" s="65"/>
+      <c r="Z27" s="65"/>
+      <c r="AA27" s="65"/>
+      <c r="AB27" s="65"/>
+      <c r="AC27" s="65"/>
+      <c r="AD27" s="65"/>
+    </row>
+    <row r="28" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="64">
         <v>26</v>
       </c>
-      <c r="G8" s="65">
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="66">
+        <v>270</v>
+      </c>
+      <c r="H28" s="66">
+        <v>271</v>
+      </c>
+      <c r="I28" s="66">
+        <v>272</v>
+      </c>
+      <c r="J28" s="65"/>
+      <c r="K28" s="65"/>
+      <c r="L28" s="65"/>
+      <c r="M28" s="67" t="s">
+        <v>149</v>
+      </c>
+      <c r="N28" s="66">
+        <v>274</v>
+      </c>
+      <c r="O28" s="65"/>
+      <c r="P28" s="65"/>
+      <c r="Q28" s="65"/>
+      <c r="R28" s="65"/>
+      <c r="S28" s="65"/>
+      <c r="T28" s="65"/>
+      <c r="U28" s="65"/>
+      <c r="V28" s="65"/>
+      <c r="W28" s="65"/>
+      <c r="X28" s="65"/>
+      <c r="Y28" s="65"/>
+      <c r="Z28" s="65"/>
+      <c r="AA28" s="65"/>
+      <c r="AB28" s="65"/>
+      <c r="AC28" s="65"/>
+      <c r="AD28" s="65"/>
+    </row>
+    <row r="29" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="64">
         <v>27</v>
       </c>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="64"/>
-      <c r="R8" s="64"/>
-      <c r="S8" s="65">
+      <c r="B29" s="65"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="66">
+        <v>275</v>
+      </c>
+      <c r="H29" s="66">
+        <v>276</v>
+      </c>
+      <c r="I29" s="66">
+        <v>277</v>
+      </c>
+      <c r="J29" s="65"/>
+      <c r="K29" s="65"/>
+      <c r="L29" s="66">
+        <v>278</v>
+      </c>
+      <c r="M29" s="66">
+        <v>279</v>
+      </c>
+      <c r="N29" s="66">
+        <v>280</v>
+      </c>
+      <c r="O29" s="66">
+        <v>281</v>
+      </c>
+      <c r="P29" s="66">
+        <v>282</v>
+      </c>
+      <c r="Q29" s="66">
+        <v>283</v>
+      </c>
+      <c r="R29" s="66">
+        <v>284</v>
+      </c>
+      <c r="S29" s="66">
+        <v>285</v>
+      </c>
+      <c r="T29" s="65"/>
+      <c r="U29" s="65"/>
+      <c r="V29" s="65"/>
+      <c r="W29" s="65"/>
+      <c r="X29" s="65"/>
+      <c r="Y29" s="65"/>
+      <c r="Z29" s="65"/>
+      <c r="AA29" s="65"/>
+      <c r="AB29" s="65"/>
+      <c r="AC29" s="65"/>
+      <c r="AD29" s="65"/>
+    </row>
+    <row r="30" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="64">
+        <v>28</v>
+      </c>
+      <c r="B30" s="65"/>
+      <c r="C30" s="65"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="66">
+        <v>286</v>
+      </c>
+      <c r="I30" s="66">
+        <v>287</v>
+      </c>
+      <c r="J30" s="65"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="65"/>
+      <c r="N30" s="65"/>
+      <c r="O30" s="65"/>
+      <c r="P30" s="65"/>
+      <c r="Q30" s="65"/>
+      <c r="R30" s="66">
+        <v>288</v>
+      </c>
+      <c r="S30" s="66">
+        <v>289</v>
+      </c>
+      <c r="T30" s="65"/>
+      <c r="U30" s="65"/>
+      <c r="V30" s="65"/>
+      <c r="W30" s="65"/>
+      <c r="X30" s="65"/>
+      <c r="Y30" s="65"/>
+      <c r="Z30" s="65"/>
+      <c r="AA30" s="65"/>
+      <c r="AB30" s="65"/>
+      <c r="AC30" s="65"/>
+      <c r="AD30" s="65"/>
+    </row>
+    <row r="31" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="64">
         <v>29</v>
       </c>
-      <c r="T8" s="65">
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="66">
+        <v>290</v>
+      </c>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="65"/>
+      <c r="L31" s="65"/>
+      <c r="M31" s="65"/>
+      <c r="N31" s="65"/>
+      <c r="O31" s="65"/>
+      <c r="P31" s="65"/>
+      <c r="Q31" s="65"/>
+      <c r="R31" s="65"/>
+      <c r="S31" s="65"/>
+      <c r="T31" s="65"/>
+      <c r="U31" s="65"/>
+      <c r="V31" s="65"/>
+      <c r="W31" s="65"/>
+      <c r="X31" s="65"/>
+      <c r="Y31" s="65"/>
+      <c r="Z31" s="65"/>
+      <c r="AA31" s="65"/>
+      <c r="AB31" s="65"/>
+      <c r="AC31" s="65"/>
+      <c r="AD31" s="65"/>
+    </row>
+    <row r="32" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="64">
         <v>30</v>
       </c>
-      <c r="U8" s="64"/>
-      <c r="V8" s="64"/>
-      <c r="W8" s="65">
+      <c r="B32" s="65"/>
+      <c r="C32" s="65"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="66">
+        <v>291</v>
+      </c>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="65"/>
+      <c r="L32" s="65"/>
+      <c r="M32" s="65"/>
+      <c r="N32" s="65"/>
+      <c r="O32" s="65"/>
+      <c r="P32" s="65"/>
+      <c r="Q32" s="65"/>
+      <c r="R32" s="65"/>
+      <c r="S32" s="65"/>
+      <c r="T32" s="65"/>
+      <c r="U32" s="65"/>
+      <c r="V32" s="65"/>
+      <c r="W32" s="65"/>
+      <c r="X32" s="65"/>
+      <c r="Y32" s="65"/>
+      <c r="Z32" s="65"/>
+      <c r="AA32" s="65"/>
+      <c r="AB32" s="65"/>
+      <c r="AC32" s="65"/>
+      <c r="AD32" s="65"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A33" s="64">
         <v>31</v>
       </c>
-      <c r="X8" s="65">
-        <v>32</v>
-      </c>
-      <c r="Y8" s="65">
-        <v>33</v>
-      </c>
-      <c r="Z8" s="64"/>
-      <c r="AA8" s="64"/>
-      <c r="AB8" s="64"/>
-      <c r="AC8" s="64"/>
-      <c r="AD8" s="64"/>
-    </row>
-    <row r="9" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="63">
-        <v>7</v>
-      </c>
-      <c r="B9" s="65">
-        <v>34</v>
-      </c>
-      <c r="C9" s="65">
-        <v>35</v>
-      </c>
-      <c r="D9" s="65">
-        <v>36</v>
-      </c>
-      <c r="E9" s="65">
-        <v>37</v>
-      </c>
-      <c r="F9" s="65">
-        <v>38</v>
-      </c>
-      <c r="G9" s="65">
-        <v>39</v>
-      </c>
-      <c r="H9" s="64"/>
-      <c r="J9" s="64"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="65">
-        <v>40</v>
-      </c>
-      <c r="N9" s="65">
-        <v>41</v>
-      </c>
-      <c r="O9" s="65">
-        <v>42</v>
-      </c>
-      <c r="P9" s="65">
-        <v>43</v>
-      </c>
-      <c r="Q9" s="65">
-        <v>44</v>
-      </c>
-      <c r="R9" s="65">
-        <v>45</v>
-      </c>
-      <c r="S9" s="65">
-        <v>46</v>
-      </c>
-      <c r="T9" s="65">
-        <v>47</v>
-      </c>
-      <c r="U9" s="65">
-        <v>48</v>
-      </c>
-      <c r="V9" s="64"/>
-      <c r="W9" s="65">
-        <v>49</v>
-      </c>
-      <c r="X9" s="65">
-        <v>50</v>
-      </c>
-      <c r="Y9" s="65">
-        <v>51</v>
-      </c>
-      <c r="Z9" s="64"/>
-      <c r="AA9" s="64"/>
-      <c r="AB9" s="64"/>
-      <c r="AC9" s="64"/>
-      <c r="AD9" s="64"/>
-    </row>
-    <row r="10" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="63">
-        <v>8</v>
-      </c>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="65">
-        <v>52</v>
-      </c>
-      <c r="G10" s="65">
-        <v>53</v>
-      </c>
-      <c r="H10" s="65">
-        <v>54</v>
-      </c>
-      <c r="I10" s="65">
-        <v>55</v>
-      </c>
-      <c r="J10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="65">
-        <v>56</v>
-      </c>
-      <c r="N10" s="65">
-        <v>57</v>
-      </c>
-      <c r="O10" s="65">
-        <v>58</v>
-      </c>
-      <c r="P10" s="65">
-        <v>59</v>
-      </c>
-      <c r="Q10" s="65">
-        <v>60</v>
-      </c>
-      <c r="R10" s="65">
-        <v>61</v>
-      </c>
-      <c r="S10" s="65">
-        <v>62</v>
-      </c>
-      <c r="T10" s="64"/>
-      <c r="U10" s="64"/>
-      <c r="V10" s="64"/>
-      <c r="W10" s="65">
-        <v>63</v>
-      </c>
-      <c r="X10" s="65">
-        <v>64</v>
-      </c>
-      <c r="Y10" s="65">
-        <v>65</v>
-      </c>
-      <c r="Z10" s="64"/>
-      <c r="AA10" s="64"/>
-      <c r="AB10" s="64"/>
-      <c r="AC10" s="64"/>
-      <c r="AD10" s="64"/>
-    </row>
-    <row r="11" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="63">
-        <v>9</v>
-      </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="65">
-        <v>66</v>
-      </c>
-      <c r="G11" s="65">
-        <v>67</v>
-      </c>
-      <c r="H11" s="65">
-        <v>68</v>
-      </c>
-      <c r="I11" s="65">
-        <v>69</v>
-      </c>
-      <c r="J11" s="65">
-        <v>70</v>
-      </c>
-      <c r="K11" s="65">
-        <v>71</v>
-      </c>
-      <c r="L11" s="65">
-        <v>72</v>
-      </c>
-      <c r="M11" s="65">
-        <v>73</v>
-      </c>
-      <c r="N11" s="65">
-        <v>74</v>
-      </c>
-      <c r="O11" s="65">
-        <v>75</v>
-      </c>
-      <c r="P11" s="65">
-        <v>76</v>
-      </c>
-      <c r="Q11" s="65">
-        <v>77</v>
-      </c>
-      <c r="R11" s="65">
-        <v>78</v>
-      </c>
-      <c r="S11" s="65">
-        <v>79</v>
-      </c>
-      <c r="T11" s="64"/>
-      <c r="U11" s="64"/>
-      <c r="V11" s="64"/>
-      <c r="W11" s="65">
-        <v>80</v>
-      </c>
-      <c r="X11" s="65">
-        <v>81</v>
-      </c>
-      <c r="Y11" s="65">
-        <v>82</v>
-      </c>
-      <c r="Z11" s="64"/>
-      <c r="AA11" s="64"/>
-      <c r="AB11" s="64"/>
-      <c r="AC11" s="64"/>
-      <c r="AD11" s="64"/>
-    </row>
-    <row r="12" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="63">
-        <v>10</v>
-      </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="65">
-        <v>83</v>
-      </c>
-      <c r="I12" s="65">
-        <v>84</v>
-      </c>
-      <c r="J12" s="65">
-        <v>85</v>
-      </c>
-      <c r="K12" s="65">
-        <v>86</v>
-      </c>
-      <c r="L12" s="65">
-        <v>87</v>
-      </c>
-      <c r="M12" s="65">
-        <v>88</v>
-      </c>
-      <c r="N12" s="65">
-        <v>89</v>
-      </c>
-      <c r="O12" s="66" t="s">
-        <v>155</v>
-      </c>
-      <c r="P12" s="66" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q12" s="65">
-        <v>92</v>
-      </c>
-      <c r="S12" s="64"/>
-      <c r="T12" s="64"/>
-      <c r="U12" s="64"/>
-      <c r="V12" s="64"/>
-      <c r="W12" s="65">
-        <v>94</v>
-      </c>
-      <c r="X12" s="65">
-        <v>95</v>
-      </c>
-      <c r="Y12" s="65">
-        <v>96</v>
-      </c>
-      <c r="Z12" s="64"/>
-      <c r="AA12" s="64"/>
-      <c r="AB12" s="64"/>
-      <c r="AC12" s="64"/>
-      <c r="AD12" s="64"/>
-    </row>
-    <row r="13" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="63">
-        <v>11</v>
-      </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="51"/>
-      <c r="L13" s="65">
-        <v>100</v>
-      </c>
-      <c r="M13" s="65">
-        <v>101</v>
-      </c>
-      <c r="N13" s="65">
-        <v>102</v>
-      </c>
-      <c r="O13" s="65">
-        <v>103</v>
-      </c>
-      <c r="P13" s="65">
-        <v>104</v>
-      </c>
-      <c r="Q13" s="65">
-        <v>105</v>
-      </c>
-      <c r="R13" s="64"/>
-      <c r="S13" s="64"/>
-      <c r="T13" s="64"/>
-      <c r="U13" s="64"/>
-      <c r="V13" s="64"/>
-      <c r="W13" s="65">
-        <v>106</v>
-      </c>
-      <c r="X13" s="65">
-        <v>107</v>
-      </c>
-      <c r="Y13" s="65">
-        <v>108</v>
-      </c>
-      <c r="Z13" s="64"/>
-      <c r="AA13" s="64"/>
-      <c r="AB13" s="64"/>
-      <c r="AC13" s="64"/>
-      <c r="AD13" s="64"/>
-    </row>
-    <row r="14" spans="1:30" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="63">
-        <v>12</v>
-      </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
-      <c r="J14" s="64"/>
-      <c r="L14" s="66" t="s">
-        <v>152</v>
-      </c>
-      <c r="M14" s="66" t="s">
-        <v>153</v>
-      </c>
-      <c r="N14" s="65">
-        <v>112</v>
-      </c>
-      <c r="O14" s="65">
-        <v>113</v>
-      </c>
-      <c r="P14" s="65">
-        <v>114</v>
-      </c>
-      <c r="Q14" s="65">
-        <v>115</v>
-      </c>
-      <c r="R14" s="65">
-        <v>116</v>
-      </c>
-      <c r="S14" s="64"/>
-      <c r="T14" s="64"/>
-      <c r="U14" s="64"/>
-      <c r="V14" s="64"/>
-      <c r="W14" s="64"/>
-      <c r="X14" s="65">
-        <v>117</v>
-      </c>
-      <c r="Y14" s="64"/>
-      <c r="Z14" s="64"/>
-      <c r="AA14" s="65">
-        <v>118</v>
-      </c>
-      <c r="AB14" s="64"/>
-      <c r="AC14" s="64"/>
-      <c r="AD14" s="64"/>
-    </row>
-    <row r="15" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="63">
-        <v>13</v>
-      </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="65">
-        <v>119</v>
-      </c>
-      <c r="M15" s="65">
-        <v>120</v>
-      </c>
-      <c r="N15" s="66" t="s">
-        <v>154</v>
-      </c>
-      <c r="O15" s="65">
-        <v>122</v>
-      </c>
-      <c r="P15" s="65">
-        <v>123</v>
-      </c>
-      <c r="Q15" s="65">
-        <v>124</v>
-      </c>
-      <c r="R15" s="65">
-        <v>125</v>
-      </c>
-      <c r="S15" s="64"/>
-      <c r="T15" s="64"/>
-      <c r="U15" s="65">
-        <v>126</v>
-      </c>
-      <c r="V15" s="65">
-        <v>127</v>
-      </c>
-      <c r="W15" s="65">
-        <v>128</v>
-      </c>
-      <c r="X15" s="65">
-        <v>129</v>
-      </c>
-      <c r="Y15" s="65">
-        <v>130</v>
-      </c>
-      <c r="Z15" s="65">
-        <v>131</v>
-      </c>
-      <c r="AA15" s="65">
-        <v>132</v>
-      </c>
-      <c r="AB15" s="64"/>
-      <c r="AC15" s="64"/>
-      <c r="AD15" s="64"/>
-    </row>
-    <row r="16" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="63">
-        <v>14</v>
-      </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="64"/>
-      <c r="K16" s="65">
-        <v>133</v>
-      </c>
-      <c r="L16" s="65">
-        <v>134</v>
-      </c>
-      <c r="M16" s="65">
-        <v>135</v>
-      </c>
-      <c r="N16" s="65">
-        <v>136</v>
-      </c>
-      <c r="O16" s="65">
-        <v>137</v>
-      </c>
-      <c r="P16" s="65">
-        <v>138</v>
-      </c>
-      <c r="Q16" s="65">
-        <v>139</v>
-      </c>
-      <c r="R16" s="65">
-        <v>140</v>
-      </c>
-      <c r="S16" s="65">
-        <v>141</v>
-      </c>
-      <c r="T16" s="65">
-        <v>142</v>
-      </c>
-      <c r="U16" s="65">
-        <v>143</v>
-      </c>
-      <c r="V16" s="65">
-        <v>144</v>
-      </c>
-      <c r="W16" s="65">
-        <v>145</v>
-      </c>
-      <c r="X16" s="65">
-        <v>146</v>
-      </c>
-      <c r="Y16" s="65">
-        <v>147</v>
-      </c>
-      <c r="Z16" s="65">
-        <v>148</v>
-      </c>
-      <c r="AA16" s="65">
-        <v>149</v>
-      </c>
-      <c r="AB16" s="65">
-        <v>150</v>
-      </c>
-      <c r="AC16" s="64"/>
-      <c r="AD16" s="64"/>
-    </row>
-    <row r="17" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="63">
-        <v>15</v>
-      </c>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="64"/>
-      <c r="J17" s="64"/>
-      <c r="K17" s="65">
-        <v>151</v>
-      </c>
-      <c r="L17" s="65">
-        <v>152</v>
-      </c>
-      <c r="M17" s="65">
-        <v>153</v>
-      </c>
-      <c r="N17" s="65">
-        <v>154</v>
-      </c>
-      <c r="O17" s="65">
-        <v>155</v>
-      </c>
-      <c r="P17" s="65">
-        <v>156</v>
-      </c>
-      <c r="Q17" s="65">
-        <v>157</v>
-      </c>
-      <c r="R17" s="65">
-        <v>158</v>
-      </c>
-      <c r="S17" s="65">
-        <v>159</v>
-      </c>
-      <c r="T17" s="65">
-        <v>160</v>
-      </c>
-      <c r="U17" s="65">
-        <v>161</v>
-      </c>
-      <c r="V17" s="65">
-        <v>162</v>
-      </c>
-      <c r="W17" s="66" t="s">
-        <v>157</v>
-      </c>
-      <c r="X17" s="65">
-        <v>164</v>
-      </c>
-      <c r="Y17" s="65">
-        <v>165</v>
-      </c>
-      <c r="Z17" s="65">
-        <v>166</v>
-      </c>
-      <c r="AA17" s="65">
-        <v>167</v>
-      </c>
-      <c r="AB17" s="65">
-        <v>168</v>
-      </c>
-      <c r="AC17" s="64"/>
-      <c r="AD17" s="64"/>
-    </row>
-    <row r="18" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="63">
-        <v>16</v>
-      </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="64"/>
-      <c r="K18" s="65">
-        <v>169</v>
-      </c>
-      <c r="L18" s="65">
-        <v>170</v>
-      </c>
-      <c r="M18" s="65">
-        <v>171</v>
-      </c>
-      <c r="N18" s="65">
-        <v>172</v>
-      </c>
-      <c r="O18" s="65">
-        <v>173</v>
-      </c>
-      <c r="P18" s="65">
-        <v>174</v>
-      </c>
-      <c r="Q18" s="64"/>
-      <c r="R18" s="65">
-        <v>175</v>
-      </c>
-      <c r="S18" s="65">
-        <v>176</v>
-      </c>
-      <c r="T18" s="65">
-        <v>177</v>
-      </c>
-      <c r="U18" s="65">
-        <v>178</v>
-      </c>
-      <c r="V18" s="65">
-        <v>179</v>
-      </c>
-      <c r="W18" s="65">
-        <v>180</v>
-      </c>
-      <c r="Y18" s="64"/>
-      <c r="Z18" s="65">
-        <v>182</v>
-      </c>
-      <c r="AA18" s="65">
-        <v>183</v>
-      </c>
-      <c r="AB18" s="65">
-        <v>184</v>
-      </c>
-      <c r="AC18" s="65">
-        <v>185</v>
-      </c>
-      <c r="AD18" s="65">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="63">
-        <v>17</v>
-      </c>
-      <c r="B19" s="64"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="64"/>
-      <c r="J19" s="64"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="65">
-        <v>187</v>
-      </c>
-      <c r="M19" s="65">
-        <v>188</v>
-      </c>
-      <c r="N19" s="65">
-        <v>189</v>
-      </c>
-      <c r="O19" s="65">
-        <v>190</v>
-      </c>
-      <c r="P19" s="64"/>
-      <c r="Q19" s="64"/>
-      <c r="R19" s="65">
-        <v>191</v>
-      </c>
-      <c r="S19" s="65">
-        <v>192</v>
-      </c>
-      <c r="T19" s="65">
-        <v>193</v>
-      </c>
-      <c r="U19" s="65">
-        <v>194</v>
-      </c>
-      <c r="V19" s="65">
-        <v>195</v>
-      </c>
-      <c r="W19" s="65">
-        <v>196</v>
-      </c>
-      <c r="X19" s="64"/>
-      <c r="Y19" s="64"/>
-      <c r="Z19" s="64"/>
-      <c r="AA19" s="64"/>
-      <c r="AB19" s="64"/>
-      <c r="AC19" s="64"/>
-      <c r="AD19" s="65">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="63">
-        <v>18</v>
-      </c>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="65">
-        <v>198</v>
-      </c>
-      <c r="M20" s="65">
-        <v>199</v>
-      </c>
-      <c r="N20" s="65">
-        <v>200</v>
-      </c>
-      <c r="O20" s="64"/>
-      <c r="P20" s="64"/>
-      <c r="Q20" s="67"/>
-      <c r="R20" s="65">
-        <v>202</v>
-      </c>
-      <c r="S20" s="65">
-        <v>203</v>
-      </c>
-      <c r="T20" s="65">
-        <v>204</v>
-      </c>
-      <c r="U20" s="65">
-        <v>205</v>
-      </c>
-      <c r="V20" s="65">
-        <v>206</v>
-      </c>
-      <c r="W20" s="65">
-        <v>207</v>
-      </c>
-      <c r="X20" s="64"/>
-      <c r="Y20" s="64"/>
-      <c r="Z20" s="64"/>
-      <c r="AA20" s="64"/>
-      <c r="AB20" s="64"/>
-      <c r="AC20" s="64"/>
-      <c r="AD20" s="64"/>
-    </row>
-    <row r="21" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="63">
-        <v>19</v>
-      </c>
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="65">
-        <v>208</v>
-      </c>
-      <c r="G21" s="65">
-        <v>209</v>
-      </c>
-      <c r="H21" s="65">
-        <v>210</v>
-      </c>
-      <c r="I21" s="65">
-        <v>211</v>
-      </c>
-      <c r="J21" s="65">
-        <v>212</v>
-      </c>
-      <c r="K21" s="65">
-        <v>213</v>
-      </c>
-      <c r="L21" s="65">
-        <v>214</v>
-      </c>
-      <c r="M21" s="64"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="64"/>
-      <c r="P21" s="64"/>
-      <c r="Q21" s="66" t="s">
-        <v>156</v>
-      </c>
-      <c r="R21" s="65">
-        <v>216</v>
-      </c>
-      <c r="S21" s="65">
-        <v>217</v>
-      </c>
-      <c r="T21" s="65">
-        <v>218</v>
-      </c>
-      <c r="U21" s="65">
-        <v>219</v>
-      </c>
-      <c r="V21" s="65">
-        <v>220</v>
-      </c>
-      <c r="W21" s="65">
-        <v>221</v>
-      </c>
-      <c r="X21" s="64"/>
-      <c r="Y21" s="64"/>
-      <c r="Z21" s="64"/>
-      <c r="AA21" s="64"/>
-      <c r="AB21" s="64"/>
-      <c r="AC21" s="64"/>
-      <c r="AD21" s="64"/>
-    </row>
-    <row r="22" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="63">
-        <v>20</v>
-      </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="65">
-        <v>222</v>
-      </c>
-      <c r="G22" s="65">
-        <v>223</v>
-      </c>
-      <c r="H22" s="65">
-        <v>224</v>
-      </c>
-      <c r="I22" s="65">
-        <v>225</v>
-      </c>
-      <c r="J22" s="65">
-        <v>226</v>
-      </c>
-      <c r="K22" s="66" t="s">
-        <v>159</v>
-      </c>
-      <c r="L22" s="64"/>
-      <c r="M22" s="64"/>
-      <c r="O22" s="64"/>
-      <c r="P22" s="64"/>
-      <c r="Q22" s="65">
-        <v>229</v>
-      </c>
-      <c r="R22" s="64"/>
-      <c r="S22" s="64"/>
-      <c r="T22" s="64"/>
-      <c r="U22" s="64"/>
-      <c r="V22" s="64"/>
-      <c r="W22" s="64"/>
-      <c r="X22" s="64"/>
-      <c r="Y22" s="64"/>
-      <c r="Z22" s="64"/>
-      <c r="AA22" s="64"/>
-      <c r="AB22" s="64"/>
-      <c r="AC22" s="64"/>
-      <c r="AD22" s="64"/>
-    </row>
-    <row r="23" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="63">
-        <v>21</v>
-      </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="65">
-        <v>230</v>
-      </c>
-      <c r="G23" s="65">
-        <v>231</v>
-      </c>
-      <c r="H23" s="65">
-        <v>232</v>
-      </c>
-      <c r="I23" s="65">
-        <v>233</v>
-      </c>
-      <c r="J23" s="65">
-        <v>234</v>
-      </c>
-      <c r="K23" s="66" t="s">
-        <v>151</v>
-      </c>
-      <c r="L23" s="51"/>
-      <c r="P23" s="65">
-        <v>237</v>
-      </c>
-      <c r="Q23" s="65">
-        <v>238</v>
-      </c>
-      <c r="R23" s="64"/>
-      <c r="S23" s="64"/>
-      <c r="T23" s="64"/>
-      <c r="V23" s="64"/>
-      <c r="W23" s="64"/>
-      <c r="X23" s="64"/>
-      <c r="Y23" s="64"/>
-      <c r="Z23" s="64"/>
-      <c r="AB23" s="64"/>
-      <c r="AC23" s="64"/>
-      <c r="AD23" s="64"/>
-    </row>
-    <row r="24" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="63">
-        <v>22</v>
-      </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="65">
-        <v>239</v>
-      </c>
-      <c r="G24" s="65">
-        <v>240</v>
-      </c>
-      <c r="H24" s="65">
-        <v>241</v>
-      </c>
-      <c r="I24" s="65">
-        <v>242</v>
-      </c>
-      <c r="J24" s="65">
-        <v>243</v>
-      </c>
-      <c r="K24" s="65">
-        <v>244</v>
-      </c>
-      <c r="P24" s="65">
-        <v>245</v>
-      </c>
-      <c r="Q24" s="64"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="64"/>
-      <c r="T24" s="64"/>
-      <c r="V24" s="64"/>
-      <c r="W24" s="64"/>
-      <c r="X24" s="64"/>
-      <c r="Y24" s="64"/>
-      <c r="Z24" s="64"/>
-      <c r="AA24" s="64"/>
-      <c r="AB24" s="64"/>
-      <c r="AC24" s="64"/>
-      <c r="AD24" s="64"/>
-    </row>
-    <row r="25" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="63">
-        <v>23</v>
-      </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="65">
-        <v>246</v>
-      </c>
-      <c r="F25" s="65">
-        <v>247</v>
-      </c>
-      <c r="G25" s="65">
-        <v>248</v>
-      </c>
-      <c r="H25" s="65">
-        <v>249</v>
-      </c>
-      <c r="I25" s="65">
-        <v>250</v>
-      </c>
-      <c r="J25" s="65">
-        <v>251</v>
-      </c>
-      <c r="K25" s="65">
-        <v>252</v>
-      </c>
-      <c r="P25" s="65">
-        <v>254</v>
-      </c>
-      <c r="Q25" s="64"/>
-      <c r="R25" s="64"/>
-      <c r="S25" s="64"/>
-      <c r="T25" s="64"/>
-      <c r="V25" s="64"/>
-      <c r="W25" s="64"/>
-      <c r="X25" s="64"/>
-      <c r="Y25" s="64"/>
-      <c r="Z25" s="64"/>
-      <c r="AA25" s="64"/>
-      <c r="AB25" s="64"/>
-      <c r="AC25" s="64"/>
-      <c r="AD25" s="64"/>
-    </row>
-    <row r="26" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="63">
-        <v>24</v>
-      </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="64"/>
-      <c r="G26" s="65">
-        <v>255</v>
-      </c>
-      <c r="H26" s="65">
-        <v>256</v>
-      </c>
-      <c r="I26" s="65">
-        <v>257</v>
-      </c>
-      <c r="J26" s="65">
-        <v>258</v>
-      </c>
-      <c r="K26" s="65">
-        <v>259</v>
-      </c>
-      <c r="L26" s="64"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="66" t="s">
-        <v>150</v>
-      </c>
-      <c r="O26" s="65">
-        <v>261</v>
-      </c>
-      <c r="P26" s="65">
-        <v>262</v>
-      </c>
-      <c r="T26" s="64"/>
-      <c r="U26" s="64"/>
-      <c r="V26" s="64"/>
-      <c r="W26" s="64"/>
-      <c r="X26" s="64"/>
-      <c r="Y26" s="64"/>
-      <c r="Z26" s="64"/>
-      <c r="AA26" s="64"/>
-      <c r="AB26" s="64"/>
-      <c r="AC26" s="64"/>
-      <c r="AD26" s="64"/>
-    </row>
-    <row r="27" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="63">
-        <v>25</v>
-      </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64"/>
-      <c r="G27" s="65">
-        <v>263</v>
-      </c>
-      <c r="H27" s="65">
-        <v>264</v>
-      </c>
-      <c r="I27" s="65">
-        <v>265</v>
-      </c>
-      <c r="J27" s="65">
-        <v>266</v>
-      </c>
-      <c r="K27" s="65">
-        <v>267</v>
-      </c>
-      <c r="L27" s="64"/>
-      <c r="N27" s="65">
-        <v>269</v>
-      </c>
-      <c r="O27" s="64"/>
-      <c r="P27" s="64"/>
-      <c r="T27" s="64"/>
-      <c r="U27" s="64"/>
-      <c r="W27" s="64"/>
-      <c r="X27" s="64"/>
-      <c r="Y27" s="64"/>
-      <c r="Z27" s="64"/>
-      <c r="AA27" s="64"/>
-      <c r="AB27" s="64"/>
-      <c r="AC27" s="64"/>
-      <c r="AD27" s="64"/>
-    </row>
-    <row r="28" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="63">
-        <v>26</v>
-      </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="65">
-        <v>270</v>
-      </c>
-      <c r="H28" s="65">
-        <v>271</v>
-      </c>
-      <c r="I28" s="65">
-        <v>272</v>
-      </c>
-      <c r="J28" s="64"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="66" t="s">
-        <v>149</v>
-      </c>
-      <c r="N28" s="65">
-        <v>274</v>
-      </c>
-      <c r="O28" s="64"/>
-      <c r="P28" s="64"/>
-      <c r="Q28" s="64"/>
-      <c r="R28" s="64"/>
-      <c r="S28" s="64"/>
-      <c r="T28" s="64"/>
-      <c r="U28" s="64"/>
-      <c r="W28" s="64"/>
-      <c r="X28" s="64"/>
-      <c r="Y28" s="64"/>
-      <c r="Z28" s="64"/>
-      <c r="AA28" s="64"/>
-      <c r="AB28" s="64"/>
-      <c r="AC28" s="64"/>
-      <c r="AD28" s="64"/>
-    </row>
-    <row r="29" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="63">
-        <v>27</v>
-      </c>
-      <c r="B29" s="64"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="65">
-        <v>275</v>
-      </c>
-      <c r="H29" s="65">
-        <v>276</v>
-      </c>
-      <c r="I29" s="65">
-        <v>277</v>
-      </c>
-      <c r="J29" s="64"/>
-      <c r="K29" s="64"/>
-      <c r="L29" s="65">
-        <v>278</v>
-      </c>
-      <c r="M29" s="65">
-        <v>279</v>
-      </c>
-      <c r="N29" s="65">
-        <v>280</v>
-      </c>
-      <c r="O29" s="65">
-        <v>281</v>
-      </c>
-      <c r="P29" s="65">
-        <v>282</v>
-      </c>
-      <c r="Q29" s="65">
-        <v>283</v>
-      </c>
-      <c r="R29" s="65">
-        <v>284</v>
-      </c>
-      <c r="S29" s="65">
-        <v>285</v>
-      </c>
-      <c r="T29" s="64"/>
-      <c r="U29" s="64"/>
-      <c r="W29" s="64"/>
-      <c r="X29" s="64"/>
-      <c r="Y29" s="64"/>
-      <c r="Z29" s="64"/>
-      <c r="AA29" s="64"/>
-      <c r="AB29" s="64"/>
-      <c r="AC29" s="64"/>
-      <c r="AD29" s="64"/>
-    </row>
-    <row r="30" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="63">
-        <v>28</v>
-      </c>
-      <c r="B30" s="64"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="65">
-        <v>286</v>
-      </c>
-      <c r="I30" s="65">
-        <v>287</v>
-      </c>
-      <c r="J30" s="64"/>
-      <c r="O30" s="64"/>
-      <c r="P30" s="64"/>
-      <c r="Q30" s="64"/>
-      <c r="R30" s="65">
-        <v>288</v>
-      </c>
-      <c r="S30" s="65">
-        <v>289</v>
-      </c>
-      <c r="T30" s="64"/>
-      <c r="U30" s="64"/>
-      <c r="V30" s="64"/>
-      <c r="W30" s="64"/>
-      <c r="X30" s="64"/>
-      <c r="Y30" s="64"/>
-      <c r="Z30" s="64"/>
-      <c r="AA30" s="64"/>
-      <c r="AB30" s="64"/>
-      <c r="AC30" s="64"/>
-      <c r="AD30" s="64"/>
-    </row>
-    <row r="31" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="63">
-        <v>29</v>
-      </c>
-      <c r="B31" s="64"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="65">
-        <v>290</v>
-      </c>
-      <c r="I31" s="64"/>
-      <c r="J31" s="64"/>
-      <c r="K31" s="64"/>
-      <c r="N31" s="64"/>
-      <c r="O31" s="64"/>
-      <c r="P31" s="64"/>
-      <c r="Q31" s="64"/>
-      <c r="R31" s="64"/>
-      <c r="S31" s="64"/>
-      <c r="T31" s="64"/>
-      <c r="U31" s="64"/>
-      <c r="V31" s="64"/>
-      <c r="W31" s="64"/>
-      <c r="X31" s="64"/>
-      <c r="Y31" s="64"/>
-      <c r="Z31" s="64"/>
-      <c r="AA31" s="64"/>
-      <c r="AB31" s="64"/>
-      <c r="AC31" s="64"/>
-      <c r="AD31" s="64"/>
-    </row>
-    <row r="32" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="63">
-        <v>30</v>
-      </c>
-      <c r="B32" s="64"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="65">
-        <v>291</v>
-      </c>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
-      <c r="K32" s="64"/>
-      <c r="N32" s="64"/>
-      <c r="O32" s="64"/>
-      <c r="P32" s="64"/>
-      <c r="Q32" s="64"/>
-      <c r="R32" s="64"/>
-      <c r="S32" s="64"/>
-      <c r="T32" s="64"/>
-      <c r="U32" s="64"/>
-      <c r="V32" s="64"/>
-      <c r="W32" s="64"/>
-      <c r="X32" s="64"/>
-      <c r="Y32" s="64"/>
-      <c r="Z32" s="64"/>
-      <c r="AA32" s="64"/>
-      <c r="AB32" s="64"/>
-      <c r="AC32" s="64"/>
-      <c r="AD32" s="64"/>
-    </row>
-    <row r="33" spans="1:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="63">
-        <v>31</v>
-      </c>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="66" t="s">
-        <v>158</v>
-      </c>
-      <c r="J33" s="64"/>
-      <c r="L33" s="64"/>
-      <c r="M33" s="64"/>
-      <c r="N33" s="64"/>
-      <c r="O33" s="64"/>
-      <c r="P33" s="64"/>
-      <c r="Q33" s="64"/>
-      <c r="R33" s="64"/>
-      <c r="S33" s="64"/>
-      <c r="T33" s="64"/>
-      <c r="U33" s="64"/>
-      <c r="V33" s="64"/>
-      <c r="W33" s="64"/>
-      <c r="X33" s="64"/>
-      <c r="Y33" s="64"/>
-      <c r="Z33" s="64"/>
-      <c r="AA33" s="64"/>
-      <c r="AB33" s="64"/>
-      <c r="AC33" s="64"/>
-      <c r="AD33" s="64"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="66">
+        <v>292</v>
+      </c>
+      <c r="I33" s="66">
+        <v>293</v>
+      </c>
+      <c r="J33" s="65"/>
+      <c r="K33" s="65"/>
+      <c r="L33" s="65"/>
+      <c r="M33" s="65"/>
+      <c r="N33" s="65"/>
+      <c r="O33" s="65"/>
+      <c r="P33" s="65"/>
+      <c r="Q33" s="65"/>
+      <c r="R33" s="65"/>
+      <c r="S33" s="65"/>
+      <c r="T33" s="65"/>
+      <c r="U33" s="65"/>
+      <c r="V33" s="65"/>
+      <c r="W33" s="65"/>
+      <c r="X33" s="65"/>
+      <c r="Y33" s="65"/>
+      <c r="Z33" s="65"/>
+      <c r="AA33" s="65"/>
+      <c r="AB33" s="65"/>
+      <c r="AC33" s="65"/>
+      <c r="AD33" s="65"/>
     </row>
     <row r="34" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="44"/>
@@ -11686,7 +11733,7 @@
   <dimension ref="A1:AU55"/>
   <sheetViews>
     <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X47" sqref="X47"/>
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11701,7 +11748,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="63" t="s">
         <v>142</v>
       </c>
       <c r="B1" s="3">
@@ -11746,7 +11793,7 @@
       <c r="O1" s="3">
         <v>26</v>
       </c>
-      <c r="Q1" s="68" t="s">
+      <c r="Q1" s="63" t="s">
         <v>140</v>
       </c>
       <c r="R1" s="3">
@@ -11791,7 +11838,7 @@
       <c r="AE1" s="3">
         <v>26</v>
       </c>
-      <c r="AG1" s="68" t="s">
+      <c r="AG1" s="63" t="s">
         <v>141</v>
       </c>
       <c r="AH1" s="3">
@@ -12824,7 +12871,7 @@
       <c r="AU17" s="40"/>
     </row>
     <row r="19" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="63" t="s">
         <v>143</v>
       </c>
       <c r="B19" s="3">
@@ -12869,7 +12916,7 @@
       <c r="O19" s="3">
         <v>26</v>
       </c>
-      <c r="Q19" s="68" t="s">
+      <c r="Q19" s="63" t="s">
         <v>144</v>
       </c>
       <c r="R19" s="3">
@@ -12914,7 +12961,7 @@
       <c r="AE19" s="3">
         <v>26</v>
       </c>
-      <c r="AG19" s="68" t="s">
+      <c r="AG19" s="63" t="s">
         <v>145</v>
       </c>
       <c r="AH19" s="3">
@@ -13961,7 +14008,7 @@
       <c r="AU35" s="40"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A37" s="68" t="s">
+      <c r="A37" s="63" t="s">
         <v>146</v>
       </c>
       <c r="B37" s="3">
@@ -14006,7 +14053,7 @@
       <c r="O37" s="3">
         <v>26</v>
       </c>
-      <c r="Q37" s="68" t="s">
+      <c r="Q37" s="63" t="s">
         <v>147</v>
       </c>
       <c r="R37" s="3">

</xml_diff>

<commit_message>
First steps to implementing first boss battle
</commit_message>
<xml_diff>
--- a/Planning/OverworldMap.xlsx
+++ b/Planning/OverworldMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Repos\ZeldasAdventureRemastered\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B9EE48-0966-4AC8-B259-CC2513AEF798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ECF175-0FC0-4B54-9A3D-04F5E6532BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{2A32EC26-D8CF-452B-B3E7-5B8DBE295FDC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{2A32EC26-D8CF-452B-B3E7-5B8DBE295FDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Music" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="186">
   <si>
     <t>Shrine_Earth_01</t>
   </si>
@@ -571,6 +571,24 @@
   </si>
   <si>
     <t>ShrineOfEarth_21_to_22</t>
+  </si>
+  <si>
+    <t>BossPosition</t>
+  </si>
+  <si>
+    <t>AddX</t>
+  </si>
+  <si>
+    <t>AddY</t>
+  </si>
+  <si>
+    <t>PosX</t>
+  </si>
+  <si>
+    <t>PosY</t>
+  </si>
+  <si>
+    <t>Shrine of Earth - Llort</t>
   </si>
 </sst>
 </file>
@@ -802,7 +820,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -890,11 +908,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1113,6 +1151,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1437,9 +1481,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43D2B7C-3585-4BA8-AFBB-6AB1B7CD5C87}">
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M37" sqref="M37"/>
+      <selection pane="topRight" activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14831,10 +14875,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B7C2B5-A3F4-4A6B-913D-2117547F5F2B}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14892,21 +14936,21 @@
         <v>12</v>
       </c>
       <c r="C2" s="40">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="71">
-        <v>4784</v>
+        <v>4812</v>
       </c>
       <c r="E2" s="71">
-        <v>7168</v>
+        <v>7292</v>
       </c>
       <c r="F2" s="40">
         <f>SUM(D2-B2*$B$4)</f>
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="G2" s="40">
         <f>SUM(E2-C2*$B$5)</f>
-        <v>208</v>
+        <v>92</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>166</v>
@@ -14922,7 +14966,7 @@
       </c>
       <c r="L2" s="4" t="str">
         <f>_xlfn.CONCAT(A2,J2,H2,B1,J2,B2,I2,C1,J2,C2,I2,F1,J2,F2,I2,G1,J2,G2,K2,I2)</f>
-        <v>ShrineOfEarth_21_to_22:{TileX:12,TileY:29,PlayerX:176,PlayerY:208},</v>
+        <v>ShrineOfEarth_21_to_22:{TileX:12,TileY:30,PlayerX:204,PlayerY:92},</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -14941,7 +14985,251 @@
         <v>240</v>
       </c>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="73" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="73" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="73" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="73" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="74" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="74" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="75" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8" s="40">
+        <v>132</v>
+      </c>
+      <c r="C8" s="40">
+        <v>50</v>
+      </c>
+      <c r="D8" s="40">
+        <v>72</v>
+      </c>
+      <c r="E8" s="40">
+        <v>42</v>
+      </c>
+      <c r="F8" s="71">
+        <f>B8+D8</f>
+        <v>204</v>
+      </c>
+      <c r="G8" s="71">
+        <f>C8+E8</f>
+        <v>92</v>
+      </c>
+      <c r="H8" s="4" t="str">
+        <f>_xlfn.CONCAT("x=",F8,", y=",G8)</f>
+        <v>x=204, y=92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="76"/>
+      <c r="B9" s="40">
+        <v>28</v>
+      </c>
+      <c r="C9" s="40">
+        <v>40</v>
+      </c>
+      <c r="D9" s="40">
+        <v>72</v>
+      </c>
+      <c r="E9" s="40">
+        <v>42</v>
+      </c>
+      <c r="F9" s="71">
+        <f t="shared" ref="F9:F15" si="0">B9+D9</f>
+        <v>100</v>
+      </c>
+      <c r="G9" s="71">
+        <f t="shared" ref="G9:G15" si="1">C9+E9</f>
+        <v>82</v>
+      </c>
+      <c r="H9" s="4" t="str">
+        <f t="shared" ref="H9:H15" si="2">_xlfn.CONCAT("x=",F9,", y=",G9)</f>
+        <v>x=100, y=82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="76"/>
+      <c r="B10" s="40">
+        <v>132</v>
+      </c>
+      <c r="C10" s="40">
+        <v>80</v>
+      </c>
+      <c r="D10" s="40">
+        <v>72</v>
+      </c>
+      <c r="E10" s="40">
+        <v>42</v>
+      </c>
+      <c r="F10" s="71">
+        <f t="shared" si="0"/>
+        <v>204</v>
+      </c>
+      <c r="G10" s="71">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="H10" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>x=204, y=122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="76"/>
+      <c r="B11" s="40">
+        <v>216</v>
+      </c>
+      <c r="C11" s="40">
+        <v>40</v>
+      </c>
+      <c r="D11" s="40">
+        <v>72</v>
+      </c>
+      <c r="E11" s="40">
+        <v>42</v>
+      </c>
+      <c r="F11" s="71">
+        <f t="shared" si="0"/>
+        <v>288</v>
+      </c>
+      <c r="G11" s="71">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="H11" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>x=288, y=82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="76"/>
+      <c r="B12" s="40">
+        <v>132</v>
+      </c>
+      <c r="C12" s="40">
+        <v>100</v>
+      </c>
+      <c r="D12" s="40">
+        <v>72</v>
+      </c>
+      <c r="E12" s="40">
+        <v>42</v>
+      </c>
+      <c r="F12" s="71">
+        <f t="shared" si="0"/>
+        <v>204</v>
+      </c>
+      <c r="G12" s="71">
+        <f t="shared" si="1"/>
+        <v>142</v>
+      </c>
+      <c r="H12" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>x=204, y=142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="76"/>
+      <c r="B13" s="40">
+        <v>228</v>
+      </c>
+      <c r="C13" s="40">
+        <v>112</v>
+      </c>
+      <c r="D13" s="40">
+        <v>72</v>
+      </c>
+      <c r="E13" s="40">
+        <v>42</v>
+      </c>
+      <c r="F13" s="71">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="G13" s="71">
+        <f t="shared" si="1"/>
+        <v>154</v>
+      </c>
+      <c r="H13" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>x=300, y=154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="76"/>
+      <c r="B14" s="40">
+        <v>40</v>
+      </c>
+      <c r="C14" s="40">
+        <v>112</v>
+      </c>
+      <c r="D14" s="40">
+        <v>72</v>
+      </c>
+      <c r="E14" s="40">
+        <v>42</v>
+      </c>
+      <c r="F14" s="71">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="G14" s="71">
+        <f t="shared" si="1"/>
+        <v>154</v>
+      </c>
+      <c r="H14" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>x=112, y=154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="76"/>
+      <c r="B15" s="40">
+        <v>132</v>
+      </c>
+      <c r="C15" s="40">
+        <v>40</v>
+      </c>
+      <c r="D15" s="40">
+        <v>72</v>
+      </c>
+      <c r="E15" s="40">
+        <v>42</v>
+      </c>
+      <c r="F15" s="71">
+        <f t="shared" si="0"/>
+        <v>204</v>
+      </c>
+      <c r="G15" s="71">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+      <c r="H15" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>x=204, y=82</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:A15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finish Plain of Andor and Forest of Findo
</commit_message>
<xml_diff>
--- a/Planning/OverworldMap.xlsx
+++ b/Planning/OverworldMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Repos\ZeldasAdventureRemastered\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21064C4-6084-4A1F-9A3A-7AE620A36978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A7E6B5-B55D-4AF9-BB65-A27B1A4F35EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31095" yWindow="3840" windowWidth="44940" windowHeight="10500" activeTab="6" xr2:uid="{2A32EC26-D8CF-452B-B3E7-5B8DBE295FDC}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{2A32EC26-D8CF-452B-B3E7-5B8DBE295FDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Music" sheetId="1" r:id="rId1"/>
@@ -1483,7 +1483,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N22" sqref="N22"/>
+      <selection pane="topRight" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14933,24 +14933,24 @@
         <v>185</v>
       </c>
       <c r="B2" s="40">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="40">
         <v>20</v>
       </c>
       <c r="D2" s="71">
-        <v>4672</v>
+        <v>3776</v>
       </c>
       <c r="E2" s="71">
-        <v>4944</v>
+        <v>4924</v>
       </c>
       <c r="F2" s="40">
         <f>SUM(D2-B2*$B$4)</f>
-        <v>64</v>
+        <v>320</v>
       </c>
       <c r="G2" s="40">
         <f>SUM(E2-C2*$B$5)</f>
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>166</v>
@@ -14966,7 +14966,7 @@
       </c>
       <c r="L2" s="4" t="str">
         <f>_xlfn.CONCAT(H2,B1,J2,B2,I2,C1,J2,C2,I2,F1,J2,F2,I2,G1,J2,G2,K2,I2)</f>
-        <v>{TileX:12,TileY:20,PlayerX:64,PlayerY:144},</v>
+        <v>{TileX:9,TileY:20,PlayerX:320,PlayerY:124},</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Great Wimbich Warps, Life Potion & Candle
</commit_message>
<xml_diff>
--- a/Planning/OverworldMap.xlsx
+++ b/Planning/OverworldMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Repos\ZeldasAdventureRemastered\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A7E6B5-B55D-4AF9-BB65-A27B1A4F35EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F27F228-CA56-407F-992C-A4F9B0B80244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{2A32EC26-D8CF-452B-B3E7-5B8DBE295FDC}"/>
   </bookViews>
@@ -1483,7 +1483,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K22" sqref="K22"/>
+      <selection pane="topRight" activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14878,7 +14878,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14933,24 +14933,24 @@
         <v>185</v>
       </c>
       <c r="B2" s="40">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="40">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D2" s="71">
-        <v>3776</v>
+        <v>2892</v>
       </c>
       <c r="E2" s="71">
-        <v>4924</v>
+        <v>2840</v>
       </c>
       <c r="F2" s="40">
         <f>SUM(D2-B2*$B$4)</f>
-        <v>320</v>
+        <v>204</v>
       </c>
       <c r="G2" s="40">
         <f>SUM(E2-C2*$B$5)</f>
-        <v>124</v>
+        <v>200</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>166</v>
@@ -14966,7 +14966,7 @@
       </c>
       <c r="L2" s="4" t="str">
         <f>_xlfn.CONCAT(H2,B1,J2,B2,I2,C1,J2,C2,I2,F1,J2,F2,I2,G1,J2,G2,K2,I2)</f>
-        <v>{TileX:9,TileY:20,PlayerX:320,PlayerY:124},</v>
+        <v>{TileX:7,TileY:11,PlayerX:204,PlayerY:200},</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Improved the World Map by color coding the overworld map...
Red = Regular tile
Yellow = Shrine entrance
Blue = Shortcut (caves)
Green = Other kinds of warps like buildings or interiors and one-room caves and stuff
Purple = Fairy fountain
Gray = Shop

And I added a cheat code to mark all tiles as visited ( numpad / )
</commit_message>
<xml_diff>
--- a/Planning/OverworldMap.xlsx
+++ b/Planning/OverworldMap.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Repos\ZeldasAdventureRemastered\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F27F228-CA56-407F-992C-A4F9B0B80244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606D60D2-BC21-4F17-871A-5647F75297A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{2A32EC26-D8CF-452B-B3E7-5B8DBE295FDC}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{2A32EC26-D8CF-452B-B3E7-5B8DBE295FDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Music" sheetId="1" r:id="rId1"/>
     <sheet name="Dialog" sheetId="2" r:id="rId2"/>
     <sheet name="WorldMap_Overworld_IDs" sheetId="3" r:id="rId3"/>
     <sheet name="WorldMap_Overworld_Layout" sheetId="6" r:id="rId4"/>
-    <sheet name="WorldMap_Underworld_IDs" sheetId="4" r:id="rId5"/>
-    <sheet name="WorldMap_Underworld_Layout" sheetId="5" r:id="rId6"/>
-    <sheet name="OffsetCalculator" sheetId="7" r:id="rId7"/>
+    <sheet name="WorldMap_Overworld_Color" sheetId="9" r:id="rId5"/>
+    <sheet name="WorldMap_Underworld_IDs" sheetId="4" r:id="rId6"/>
+    <sheet name="WorldMap_Underworld_Layout" sheetId="5" r:id="rId7"/>
+    <sheet name="OffsetCalculator" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="187">
   <si>
     <t>Shrine_Earth_01</t>
   </si>
@@ -495,9 +496,6 @@
     <t>99 111</t>
   </si>
   <si>
-    <t>109 121</t>
-  </si>
-  <si>
     <t>28 90</t>
   </si>
   <si>
@@ -589,13 +587,19 @@
   </si>
   <si>
     <t>ShrineOfEarth_20_to_21</t>
+  </si>
+  <si>
+    <t>292  293</t>
+  </si>
+  <si>
+    <t>109 120</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -637,8 +641,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="31">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -819,6 +831,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA91010"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDB9326"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2782A1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF688E00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9D5BAD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF757575"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -932,7 +980,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1152,6 +1200,42 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="33" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="31" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="32" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="34" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="35" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="36" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1166,6 +1250,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF757575"/>
+      <color rgb="FF688E00"/>
+      <color rgb="FFA91010"/>
+      <color rgb="FFDB9326"/>
+      <color rgb="FF9D5BAD"/>
+      <color rgb="FF9B6F54"/>
+      <color rgb="FF2782A1"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FF00CC99"/>
       <color rgb="FFFF66FF"/>
@@ -6426,7 +6517,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I32" sqref="I32"/>
+      <selection pane="topRight" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8472,9 +8563,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C60D82-0D39-41C8-82A6-6A9D39131FF7}">
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I32" sqref="I32"/>
+      <selection pane="topRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8805,7 +8896,7 @@
         <v>15</v>
       </c>
       <c r="U7" s="67" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="V7" s="65"/>
       <c r="W7" s="66">
@@ -9115,10 +9206,10 @@
         <v>89</v>
       </c>
       <c r="O12" s="67" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="P12" s="67" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q12" s="66">
         <v>92</v>
@@ -9264,11 +9355,11 @@
       <c r="L15" s="66">
         <v>119</v>
       </c>
-      <c r="M15" s="66">
-        <v>120</v>
-      </c>
-      <c r="N15" s="67" t="s">
-        <v>154</v>
+      <c r="M15" s="67" t="s">
+        <v>186</v>
+      </c>
+      <c r="N15" s="66">
+        <v>121</v>
       </c>
       <c r="O15" s="66">
         <v>122</v>
@@ -9429,7 +9520,7 @@
         <v>162</v>
       </c>
       <c r="W17" s="67" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="X17" s="66">
         <v>164</v>
@@ -9659,7 +9750,7 @@
       <c r="O21" s="65"/>
       <c r="P21" s="65"/>
       <c r="Q21" s="67" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R21" s="66">
         <v>216</v>
@@ -9711,7 +9802,7 @@
         <v>226</v>
       </c>
       <c r="K22" s="67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L22" s="65"/>
       <c r="M22" s="65"/>
@@ -10193,7 +10284,7 @@
       <c r="AC32" s="65"/>
       <c r="AD32" s="65"/>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="64">
         <v>31</v>
       </c>
@@ -10203,12 +10294,10 @@
       <c r="E33" s="65"/>
       <c r="F33" s="65"/>
       <c r="G33" s="65"/>
-      <c r="H33" s="66">
-        <v>292</v>
-      </c>
-      <c r="I33" s="66">
-        <v>293</v>
-      </c>
+      <c r="H33" s="67" t="s">
+        <v>185</v>
+      </c>
+      <c r="I33" s="68"/>
       <c r="J33" s="65"/>
       <c r="K33" s="65"/>
       <c r="L33" s="65"/>
@@ -10478,6 +10567,2013 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A283EA-E136-4164-BE4B-388B47B94988}">
+  <dimension ref="A1:AD45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V15" sqref="V15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" style="77"/>
+    <col min="2" max="10" width="6.7109375" style="48"/>
+    <col min="11" max="11" width="6.7109375" style="48" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" style="48" customWidth="1"/>
+    <col min="13" max="14" width="6.7109375" style="48"/>
+    <col min="15" max="15" width="5" style="48" customWidth="1"/>
+    <col min="16" max="16" width="4.42578125" style="48" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="6.7109375" style="48"/>
+    <col min="21" max="21" width="4.28515625" style="48" customWidth="1"/>
+    <col min="22" max="16384" width="6.7109375" style="48"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" s="77" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="75"/>
+      <c r="B1" s="75">
+        <v>0</v>
+      </c>
+      <c r="C1" s="75">
+        <v>1</v>
+      </c>
+      <c r="D1" s="75">
+        <v>2</v>
+      </c>
+      <c r="E1" s="75">
+        <v>3</v>
+      </c>
+      <c r="F1" s="75">
+        <v>4</v>
+      </c>
+      <c r="G1" s="75">
+        <v>5</v>
+      </c>
+      <c r="H1" s="75">
+        <v>6</v>
+      </c>
+      <c r="I1" s="75">
+        <v>7</v>
+      </c>
+      <c r="J1" s="75">
+        <v>8</v>
+      </c>
+      <c r="K1" s="75">
+        <v>9</v>
+      </c>
+      <c r="L1" s="75">
+        <v>10</v>
+      </c>
+      <c r="M1" s="75">
+        <v>11</v>
+      </c>
+      <c r="N1" s="75">
+        <v>12</v>
+      </c>
+      <c r="O1" s="75">
+        <v>13</v>
+      </c>
+      <c r="P1" s="75">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="75">
+        <v>15</v>
+      </c>
+      <c r="R1" s="75">
+        <v>16</v>
+      </c>
+      <c r="S1" s="75">
+        <v>17</v>
+      </c>
+      <c r="T1" s="75">
+        <v>18</v>
+      </c>
+      <c r="U1" s="75">
+        <v>19</v>
+      </c>
+      <c r="V1" s="75">
+        <v>20</v>
+      </c>
+      <c r="W1" s="75">
+        <v>21</v>
+      </c>
+      <c r="X1" s="75">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="75">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="75">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="75">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="75">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="75">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="75">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="75">
+        <v>0</v>
+      </c>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
+      <c r="V2" s="78"/>
+      <c r="W2" s="78"/>
+      <c r="X2" s="78"/>
+      <c r="Y2" s="78"/>
+      <c r="Z2" s="78"/>
+      <c r="AA2" s="80">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="78"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
+    </row>
+    <row r="3" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="75">
+        <v>1</v>
+      </c>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78"/>
+      <c r="R3" s="78"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="78"/>
+      <c r="V3" s="78"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="78"/>
+      <c r="Z3" s="78"/>
+      <c r="AA3" s="80">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="78"/>
+      <c r="AC3" s="78"/>
+      <c r="AD3" s="78"/>
+    </row>
+    <row r="4" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="75">
+        <v>2</v>
+      </c>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="78"/>
+      <c r="R4" s="78"/>
+      <c r="S4" s="78"/>
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="78"/>
+      <c r="X4" s="78"/>
+      <c r="Y4" s="78"/>
+      <c r="Z4" s="80">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="80">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="78"/>
+      <c r="AC4" s="78"/>
+      <c r="AD4" s="78"/>
+    </row>
+    <row r="5" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="75">
+        <v>3</v>
+      </c>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="78"/>
+      <c r="M5" s="78"/>
+      <c r="N5" s="78"/>
+      <c r="O5" s="78"/>
+      <c r="P5" s="78"/>
+      <c r="Q5" s="78"/>
+      <c r="R5" s="78"/>
+      <c r="S5" s="78"/>
+      <c r="T5" s="78"/>
+      <c r="U5" s="78"/>
+      <c r="V5" s="78"/>
+      <c r="W5" s="78"/>
+      <c r="X5" s="78"/>
+      <c r="Y5" s="78"/>
+      <c r="Z5" s="80">
+        <v>4</v>
+      </c>
+      <c r="AA5" s="80">
+        <v>5</v>
+      </c>
+      <c r="AB5" s="78"/>
+      <c r="AC5" s="78"/>
+      <c r="AD5" s="78"/>
+    </row>
+    <row r="6" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="75">
+        <v>4</v>
+      </c>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="78"/>
+      <c r="M6" s="78"/>
+      <c r="N6" s="78"/>
+      <c r="O6" s="78"/>
+      <c r="P6" s="78"/>
+      <c r="Q6" s="78"/>
+      <c r="R6" s="78"/>
+      <c r="S6" s="80">
+        <v>6</v>
+      </c>
+      <c r="T6" s="81">
+        <v>7</v>
+      </c>
+      <c r="U6" s="78"/>
+      <c r="V6" s="78"/>
+      <c r="W6" s="79">
+        <v>9</v>
+      </c>
+      <c r="X6" s="80">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="80">
+        <v>11</v>
+      </c>
+      <c r="Z6" s="80">
+        <v>12</v>
+      </c>
+      <c r="AA6" s="81">
+        <v>13</v>
+      </c>
+      <c r="AB6" s="78"/>
+      <c r="AC6" s="78"/>
+      <c r="AD6" s="78"/>
+    </row>
+    <row r="7" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="75">
+        <v>5</v>
+      </c>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="78"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="78"/>
+      <c r="M7" s="78"/>
+      <c r="N7" s="78"/>
+      <c r="O7" s="78"/>
+      <c r="P7" s="78"/>
+      <c r="Q7" s="78"/>
+      <c r="R7" s="78"/>
+      <c r="S7" s="80">
+        <v>14</v>
+      </c>
+      <c r="T7" s="80">
+        <v>15</v>
+      </c>
+      <c r="U7" s="79" t="s">
+        <v>159</v>
+      </c>
+      <c r="V7" s="78"/>
+      <c r="W7" s="80">
+        <v>17</v>
+      </c>
+      <c r="X7" s="80">
+        <v>18</v>
+      </c>
+      <c r="Y7" s="80">
+        <v>19</v>
+      </c>
+      <c r="Z7" s="80">
+        <v>20</v>
+      </c>
+      <c r="AA7" s="80">
+        <v>21</v>
+      </c>
+      <c r="AB7" s="78"/>
+      <c r="AC7" s="78"/>
+      <c r="AD7" s="78"/>
+    </row>
+    <row r="8" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="75">
+        <v>6</v>
+      </c>
+      <c r="B8" s="80">
+        <v>22</v>
+      </c>
+      <c r="C8" s="81">
+        <v>23</v>
+      </c>
+      <c r="D8" s="80">
+        <v>24</v>
+      </c>
+      <c r="E8" s="80">
+        <v>25</v>
+      </c>
+      <c r="F8" s="86">
+        <v>26</v>
+      </c>
+      <c r="G8" s="80">
+        <v>27</v>
+      </c>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
+      <c r="L8" s="78"/>
+      <c r="M8" s="78"/>
+      <c r="N8" s="78"/>
+      <c r="O8" s="78"/>
+      <c r="P8" s="78"/>
+      <c r="Q8" s="78"/>
+      <c r="R8" s="78"/>
+      <c r="S8" s="80">
+        <v>29</v>
+      </c>
+      <c r="T8" s="80">
+        <v>30</v>
+      </c>
+      <c r="U8" s="78"/>
+      <c r="V8" s="78"/>
+      <c r="W8" s="80">
+        <v>31</v>
+      </c>
+      <c r="X8" s="80">
+        <v>32</v>
+      </c>
+      <c r="Y8" s="80">
+        <v>33</v>
+      </c>
+      <c r="Z8" s="78"/>
+      <c r="AA8" s="78"/>
+      <c r="AB8" s="78"/>
+      <c r="AC8" s="78"/>
+      <c r="AD8" s="78"/>
+    </row>
+    <row r="9" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="75">
+        <v>7</v>
+      </c>
+      <c r="B9" s="80">
+        <v>34</v>
+      </c>
+      <c r="C9" s="80">
+        <v>35</v>
+      </c>
+      <c r="D9" s="80">
+        <v>36</v>
+      </c>
+      <c r="E9" s="80">
+        <v>37</v>
+      </c>
+      <c r="F9" s="80">
+        <v>38</v>
+      </c>
+      <c r="G9" s="80">
+        <v>39</v>
+      </c>
+      <c r="H9" s="78"/>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78"/>
+      <c r="M9" s="81">
+        <v>40</v>
+      </c>
+      <c r="N9" s="80">
+        <v>41</v>
+      </c>
+      <c r="O9" s="80">
+        <v>42</v>
+      </c>
+      <c r="P9" s="80">
+        <v>43</v>
+      </c>
+      <c r="Q9" s="80">
+        <v>44</v>
+      </c>
+      <c r="R9" s="80">
+        <v>45</v>
+      </c>
+      <c r="S9" s="80">
+        <v>46</v>
+      </c>
+      <c r="T9" s="80">
+        <v>47</v>
+      </c>
+      <c r="U9" s="80">
+        <v>48</v>
+      </c>
+      <c r="V9" s="78"/>
+      <c r="W9" s="80">
+        <v>49</v>
+      </c>
+      <c r="X9" s="83">
+        <v>50</v>
+      </c>
+      <c r="Y9" s="80">
+        <v>51</v>
+      </c>
+      <c r="Z9" s="78"/>
+      <c r="AA9" s="78"/>
+      <c r="AB9" s="78"/>
+      <c r="AC9" s="78"/>
+      <c r="AD9" s="78"/>
+    </row>
+    <row r="10" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="75">
+        <v>8</v>
+      </c>
+      <c r="B10" s="78"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="80">
+        <v>52</v>
+      </c>
+      <c r="G10" s="80">
+        <v>53</v>
+      </c>
+      <c r="H10" s="80">
+        <v>54</v>
+      </c>
+      <c r="I10" s="80">
+        <v>55</v>
+      </c>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78"/>
+      <c r="M10" s="80">
+        <v>56</v>
+      </c>
+      <c r="N10" s="80">
+        <v>57</v>
+      </c>
+      <c r="O10" s="83">
+        <v>58</v>
+      </c>
+      <c r="P10" s="80">
+        <v>59</v>
+      </c>
+      <c r="Q10" s="80">
+        <v>60</v>
+      </c>
+      <c r="R10" s="80">
+        <v>61</v>
+      </c>
+      <c r="S10" s="80">
+        <v>62</v>
+      </c>
+      <c r="T10" s="78"/>
+      <c r="U10" s="78"/>
+      <c r="V10" s="78"/>
+      <c r="W10" s="80">
+        <v>63</v>
+      </c>
+      <c r="X10" s="80">
+        <v>64</v>
+      </c>
+      <c r="Y10" s="80">
+        <v>65</v>
+      </c>
+      <c r="Z10" s="78"/>
+      <c r="AA10" s="78"/>
+      <c r="AB10" s="78"/>
+      <c r="AC10" s="78"/>
+      <c r="AD10" s="78"/>
+    </row>
+    <row r="11" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="75">
+        <v>9</v>
+      </c>
+      <c r="B11" s="78"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="80">
+        <v>66</v>
+      </c>
+      <c r="G11" s="80">
+        <v>67</v>
+      </c>
+      <c r="H11" s="80">
+        <v>68</v>
+      </c>
+      <c r="I11" s="80">
+        <v>69</v>
+      </c>
+      <c r="J11" s="80">
+        <v>70</v>
+      </c>
+      <c r="K11" s="80">
+        <v>71</v>
+      </c>
+      <c r="L11" s="80">
+        <v>72</v>
+      </c>
+      <c r="M11" s="80">
+        <v>73</v>
+      </c>
+      <c r="N11" s="80">
+        <v>74</v>
+      </c>
+      <c r="O11" s="80">
+        <v>75</v>
+      </c>
+      <c r="P11" s="80">
+        <v>76</v>
+      </c>
+      <c r="Q11" s="80">
+        <v>77</v>
+      </c>
+      <c r="R11" s="80">
+        <v>78</v>
+      </c>
+      <c r="S11" s="80">
+        <v>79</v>
+      </c>
+      <c r="T11" s="78"/>
+      <c r="U11" s="78"/>
+      <c r="V11" s="78"/>
+      <c r="W11" s="80">
+        <v>80</v>
+      </c>
+      <c r="X11" s="80">
+        <v>81</v>
+      </c>
+      <c r="Y11" s="80">
+        <v>82</v>
+      </c>
+      <c r="Z11" s="78"/>
+      <c r="AA11" s="78"/>
+      <c r="AB11" s="78"/>
+      <c r="AC11" s="78"/>
+      <c r="AD11" s="78"/>
+    </row>
+    <row r="12" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="75">
+        <v>10</v>
+      </c>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="80">
+        <v>83</v>
+      </c>
+      <c r="I12" s="80">
+        <v>84</v>
+      </c>
+      <c r="J12" s="80">
+        <v>85</v>
+      </c>
+      <c r="K12" s="80">
+        <v>86</v>
+      </c>
+      <c r="L12" s="80">
+        <v>87</v>
+      </c>
+      <c r="M12" s="80">
+        <v>88</v>
+      </c>
+      <c r="N12" s="80">
+        <v>89</v>
+      </c>
+      <c r="O12" s="82" t="s">
+        <v>154</v>
+      </c>
+      <c r="P12" s="82" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q12" s="80">
+        <v>92</v>
+      </c>
+      <c r="R12" s="78"/>
+      <c r="S12" s="78"/>
+      <c r="T12" s="78"/>
+      <c r="U12" s="78"/>
+      <c r="V12" s="78"/>
+      <c r="W12" s="80">
+        <v>94</v>
+      </c>
+      <c r="X12" s="80">
+        <v>95</v>
+      </c>
+      <c r="Y12" s="80">
+        <v>96</v>
+      </c>
+      <c r="Z12" s="78"/>
+      <c r="AA12" s="78"/>
+      <c r="AB12" s="78"/>
+      <c r="AC12" s="78"/>
+      <c r="AD12" s="78"/>
+    </row>
+    <row r="13" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="75">
+        <v>11</v>
+      </c>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="78"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="80">
+        <v>100</v>
+      </c>
+      <c r="M13" s="80">
+        <v>101</v>
+      </c>
+      <c r="N13" s="80">
+        <v>102</v>
+      </c>
+      <c r="O13" s="80">
+        <v>103</v>
+      </c>
+      <c r="P13" s="80">
+        <v>104</v>
+      </c>
+      <c r="Q13" s="86">
+        <v>105</v>
+      </c>
+      <c r="R13" s="78"/>
+      <c r="S13" s="78"/>
+      <c r="T13" s="78"/>
+      <c r="U13" s="78"/>
+      <c r="V13" s="78"/>
+      <c r="W13" s="80">
+        <v>106</v>
+      </c>
+      <c r="X13" s="80">
+        <v>107</v>
+      </c>
+      <c r="Y13" s="80">
+        <v>108</v>
+      </c>
+      <c r="Z13" s="78"/>
+      <c r="AA13" s="78"/>
+      <c r="AB13" s="78"/>
+      <c r="AC13" s="78"/>
+      <c r="AD13" s="78"/>
+    </row>
+    <row r="14" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="75">
+        <v>12</v>
+      </c>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="82" t="s">
+        <v>152</v>
+      </c>
+      <c r="M14" s="82" t="s">
+        <v>153</v>
+      </c>
+      <c r="N14" s="80">
+        <v>112</v>
+      </c>
+      <c r="O14" s="80">
+        <v>113</v>
+      </c>
+      <c r="P14" s="80">
+        <v>114</v>
+      </c>
+      <c r="Q14" s="80">
+        <v>115</v>
+      </c>
+      <c r="R14" s="80">
+        <v>116</v>
+      </c>
+      <c r="S14" s="78"/>
+      <c r="T14" s="78"/>
+      <c r="U14" s="78"/>
+      <c r="V14" s="78"/>
+      <c r="W14" s="78"/>
+      <c r="X14" s="80">
+        <v>117</v>
+      </c>
+      <c r="Y14" s="78"/>
+      <c r="Z14" s="78"/>
+      <c r="AA14" s="80">
+        <v>118</v>
+      </c>
+      <c r="AB14" s="78"/>
+      <c r="AC14" s="78"/>
+      <c r="AD14" s="78"/>
+    </row>
+    <row r="15" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="75">
+        <v>13</v>
+      </c>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="78"/>
+      <c r="L15" s="86">
+        <v>119</v>
+      </c>
+      <c r="M15" s="84" t="s">
+        <v>186</v>
+      </c>
+      <c r="N15" s="85">
+        <v>121</v>
+      </c>
+      <c r="O15" s="80">
+        <v>122</v>
+      </c>
+      <c r="P15" s="80">
+        <v>123</v>
+      </c>
+      <c r="Q15" s="80">
+        <v>124</v>
+      </c>
+      <c r="R15" s="80">
+        <v>125</v>
+      </c>
+      <c r="S15" s="78"/>
+      <c r="T15" s="78"/>
+      <c r="U15" s="80">
+        <v>126</v>
+      </c>
+      <c r="V15" s="80">
+        <v>127</v>
+      </c>
+      <c r="W15" s="86">
+        <v>128</v>
+      </c>
+      <c r="X15" s="80">
+        <v>129</v>
+      </c>
+      <c r="Y15" s="80">
+        <v>130</v>
+      </c>
+      <c r="Z15" s="80">
+        <v>131</v>
+      </c>
+      <c r="AA15" s="80">
+        <v>132</v>
+      </c>
+      <c r="AB15" s="78"/>
+      <c r="AC15" s="78"/>
+      <c r="AD15" s="78"/>
+    </row>
+    <row r="16" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="75">
+        <v>14</v>
+      </c>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
+      <c r="H16" s="78"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="80">
+        <v>133</v>
+      </c>
+      <c r="L16" s="80">
+        <v>134</v>
+      </c>
+      <c r="M16" s="80">
+        <v>135</v>
+      </c>
+      <c r="N16" s="80">
+        <v>136</v>
+      </c>
+      <c r="O16" s="80">
+        <v>137</v>
+      </c>
+      <c r="P16" s="80">
+        <v>138</v>
+      </c>
+      <c r="Q16" s="80">
+        <v>139</v>
+      </c>
+      <c r="R16" s="80">
+        <v>140</v>
+      </c>
+      <c r="S16" s="80">
+        <v>141</v>
+      </c>
+      <c r="T16" s="80">
+        <v>142</v>
+      </c>
+      <c r="U16" s="80">
+        <v>143</v>
+      </c>
+      <c r="V16" s="80">
+        <v>144</v>
+      </c>
+      <c r="W16" s="80">
+        <v>145</v>
+      </c>
+      <c r="X16" s="80">
+        <v>146</v>
+      </c>
+      <c r="Y16" s="80">
+        <v>147</v>
+      </c>
+      <c r="Z16" s="80">
+        <v>148</v>
+      </c>
+      <c r="AA16" s="80">
+        <v>149</v>
+      </c>
+      <c r="AB16" s="80">
+        <v>150</v>
+      </c>
+      <c r="AC16" s="78"/>
+      <c r="AD16" s="78"/>
+    </row>
+    <row r="17" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="75">
+        <v>15</v>
+      </c>
+      <c r="B17" s="78"/>
+      <c r="C17" s="78"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="78"/>
+      <c r="H17" s="78"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="80">
+        <v>151</v>
+      </c>
+      <c r="L17" s="80">
+        <v>152</v>
+      </c>
+      <c r="M17" s="80">
+        <v>153</v>
+      </c>
+      <c r="N17" s="80">
+        <v>154</v>
+      </c>
+      <c r="O17" s="80">
+        <v>155</v>
+      </c>
+      <c r="P17" s="80">
+        <v>156</v>
+      </c>
+      <c r="Q17" s="80">
+        <v>157</v>
+      </c>
+      <c r="R17" s="80">
+        <v>158</v>
+      </c>
+      <c r="S17" s="80">
+        <v>159</v>
+      </c>
+      <c r="T17" s="80">
+        <v>160</v>
+      </c>
+      <c r="U17" s="80">
+        <v>161</v>
+      </c>
+      <c r="V17" s="80">
+        <v>162</v>
+      </c>
+      <c r="W17" s="82" t="s">
+        <v>156</v>
+      </c>
+      <c r="X17" s="80">
+        <v>164</v>
+      </c>
+      <c r="Y17" s="80">
+        <v>165</v>
+      </c>
+      <c r="Z17" s="80">
+        <v>166</v>
+      </c>
+      <c r="AA17" s="80">
+        <v>167</v>
+      </c>
+      <c r="AB17" s="80">
+        <v>168</v>
+      </c>
+      <c r="AC17" s="78"/>
+      <c r="AD17" s="78"/>
+    </row>
+    <row r="18" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="75">
+        <v>16</v>
+      </c>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="78"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="78"/>
+      <c r="H18" s="78"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="78"/>
+      <c r="K18" s="80">
+        <v>169</v>
+      </c>
+      <c r="L18" s="80">
+        <v>170</v>
+      </c>
+      <c r="M18" s="80">
+        <v>171</v>
+      </c>
+      <c r="N18" s="80">
+        <v>172</v>
+      </c>
+      <c r="O18" s="80">
+        <v>173</v>
+      </c>
+      <c r="P18" s="80">
+        <v>174</v>
+      </c>
+      <c r="Q18" s="78"/>
+      <c r="R18" s="80">
+        <v>175</v>
+      </c>
+      <c r="S18" s="80">
+        <v>176</v>
+      </c>
+      <c r="T18" s="80">
+        <v>177</v>
+      </c>
+      <c r="U18" s="80">
+        <v>178</v>
+      </c>
+      <c r="V18" s="80">
+        <v>179</v>
+      </c>
+      <c r="W18" s="80">
+        <v>180</v>
+      </c>
+      <c r="X18" s="78"/>
+      <c r="Y18" s="78"/>
+      <c r="Z18" s="80">
+        <v>182</v>
+      </c>
+      <c r="AA18" s="80">
+        <v>183</v>
+      </c>
+      <c r="AB18" s="80">
+        <v>184</v>
+      </c>
+      <c r="AC18" s="81">
+        <v>185</v>
+      </c>
+      <c r="AD18" s="80">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="75">
+        <v>17</v>
+      </c>
+      <c r="B19" s="78"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="78"/>
+      <c r="H19" s="78"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
+      <c r="L19" s="80">
+        <v>187</v>
+      </c>
+      <c r="M19" s="80">
+        <v>188</v>
+      </c>
+      <c r="N19" s="80">
+        <v>189</v>
+      </c>
+      <c r="O19" s="80">
+        <v>190</v>
+      </c>
+      <c r="P19" s="78"/>
+      <c r="Q19" s="78"/>
+      <c r="R19" s="80">
+        <v>191</v>
+      </c>
+      <c r="S19" s="80">
+        <v>192</v>
+      </c>
+      <c r="T19" s="80">
+        <v>193</v>
+      </c>
+      <c r="U19" s="80">
+        <v>194</v>
+      </c>
+      <c r="V19" s="80">
+        <v>195</v>
+      </c>
+      <c r="W19" s="80">
+        <v>196</v>
+      </c>
+      <c r="X19" s="78"/>
+      <c r="Y19" s="78"/>
+      <c r="Z19" s="78"/>
+      <c r="AA19" s="78"/>
+      <c r="AB19" s="78"/>
+      <c r="AC19" s="78"/>
+      <c r="AD19" s="83">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="75">
+        <v>18</v>
+      </c>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="78"/>
+      <c r="E20" s="78"/>
+      <c r="F20" s="78"/>
+      <c r="G20" s="78"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="80">
+        <v>198</v>
+      </c>
+      <c r="M20" s="80">
+        <v>199</v>
+      </c>
+      <c r="N20" s="80">
+        <v>200</v>
+      </c>
+      <c r="O20" s="78"/>
+      <c r="P20" s="78"/>
+      <c r="Q20" s="78"/>
+      <c r="R20" s="80">
+        <v>202</v>
+      </c>
+      <c r="S20" s="80">
+        <v>203</v>
+      </c>
+      <c r="T20" s="80">
+        <v>204</v>
+      </c>
+      <c r="U20" s="80">
+        <v>205</v>
+      </c>
+      <c r="V20" s="80">
+        <v>206</v>
+      </c>
+      <c r="W20" s="80">
+        <v>207</v>
+      </c>
+      <c r="X20" s="78"/>
+      <c r="Y20" s="78"/>
+      <c r="Z20" s="78"/>
+      <c r="AA20" s="78"/>
+      <c r="AB20" s="78"/>
+      <c r="AC20" s="78"/>
+      <c r="AD20" s="78"/>
+    </row>
+    <row r="21" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="75">
+        <v>19</v>
+      </c>
+      <c r="B21" s="78"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="78"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="80">
+        <v>208</v>
+      </c>
+      <c r="G21" s="80">
+        <v>209</v>
+      </c>
+      <c r="H21" s="80">
+        <v>210</v>
+      </c>
+      <c r="I21" s="80">
+        <v>211</v>
+      </c>
+      <c r="J21" s="80">
+        <v>212</v>
+      </c>
+      <c r="K21" s="80">
+        <v>213</v>
+      </c>
+      <c r="L21" s="80">
+        <v>214</v>
+      </c>
+      <c r="M21" s="78"/>
+      <c r="N21" s="78"/>
+      <c r="O21" s="78"/>
+      <c r="P21" s="78"/>
+      <c r="Q21" s="82" t="s">
+        <v>155</v>
+      </c>
+      <c r="R21" s="80">
+        <v>216</v>
+      </c>
+      <c r="S21" s="80">
+        <v>217</v>
+      </c>
+      <c r="T21" s="80">
+        <v>218</v>
+      </c>
+      <c r="U21" s="86">
+        <v>219</v>
+      </c>
+      <c r="V21" s="80">
+        <v>220</v>
+      </c>
+      <c r="W21" s="80">
+        <v>221</v>
+      </c>
+      <c r="X21" s="78"/>
+      <c r="Y21" s="78"/>
+      <c r="Z21" s="78"/>
+      <c r="AA21" s="78"/>
+      <c r="AB21" s="78"/>
+      <c r="AC21" s="78"/>
+      <c r="AD21" s="78"/>
+    </row>
+    <row r="22" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="75">
+        <v>20</v>
+      </c>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
+      <c r="D22" s="78"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="80">
+        <v>222</v>
+      </c>
+      <c r="G22" s="80">
+        <v>223</v>
+      </c>
+      <c r="H22" s="80">
+        <v>224</v>
+      </c>
+      <c r="I22" s="80">
+        <v>225</v>
+      </c>
+      <c r="J22" s="80">
+        <v>226</v>
+      </c>
+      <c r="K22" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="L22" s="78"/>
+      <c r="M22" s="78"/>
+      <c r="N22" s="78"/>
+      <c r="O22" s="78"/>
+      <c r="P22" s="78"/>
+      <c r="Q22" s="80">
+        <v>229</v>
+      </c>
+      <c r="R22" s="78"/>
+      <c r="S22" s="78"/>
+      <c r="T22" s="78"/>
+      <c r="U22" s="78"/>
+      <c r="V22" s="78"/>
+      <c r="W22" s="78"/>
+      <c r="X22" s="78"/>
+      <c r="Y22" s="78"/>
+      <c r="Z22" s="78"/>
+      <c r="AA22" s="78"/>
+      <c r="AB22" s="78"/>
+      <c r="AC22" s="78"/>
+      <c r="AD22" s="78"/>
+    </row>
+    <row r="23" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="75">
+        <v>21</v>
+      </c>
+      <c r="B23" s="78"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="80">
+        <v>230</v>
+      </c>
+      <c r="G23" s="80">
+        <v>231</v>
+      </c>
+      <c r="H23" s="80">
+        <v>232</v>
+      </c>
+      <c r="I23" s="80">
+        <v>233</v>
+      </c>
+      <c r="J23" s="80">
+        <v>234</v>
+      </c>
+      <c r="K23" s="82" t="s">
+        <v>151</v>
+      </c>
+      <c r="L23" s="78"/>
+      <c r="M23" s="78"/>
+      <c r="N23" s="78"/>
+      <c r="O23" s="78"/>
+      <c r="P23" s="79">
+        <v>237</v>
+      </c>
+      <c r="Q23" s="80">
+        <v>238</v>
+      </c>
+      <c r="R23" s="78"/>
+      <c r="S23" s="78"/>
+      <c r="T23" s="78"/>
+      <c r="U23" s="78"/>
+      <c r="V23" s="78"/>
+      <c r="W23" s="78"/>
+      <c r="X23" s="78"/>
+      <c r="Y23" s="78"/>
+      <c r="Z23" s="78"/>
+      <c r="AA23" s="78"/>
+      <c r="AB23" s="78"/>
+      <c r="AC23" s="78"/>
+      <c r="AD23" s="78"/>
+    </row>
+    <row r="24" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="75">
+        <v>22</v>
+      </c>
+      <c r="B24" s="78"/>
+      <c r="C24" s="78"/>
+      <c r="D24" s="78"/>
+      <c r="E24" s="78"/>
+      <c r="F24" s="80">
+        <v>239</v>
+      </c>
+      <c r="G24" s="80">
+        <v>240</v>
+      </c>
+      <c r="H24" s="80">
+        <v>241</v>
+      </c>
+      <c r="I24" s="80">
+        <v>242</v>
+      </c>
+      <c r="J24" s="80">
+        <v>243</v>
+      </c>
+      <c r="K24" s="80">
+        <v>244</v>
+      </c>
+      <c r="L24" s="78"/>
+      <c r="M24" s="78"/>
+      <c r="N24" s="78"/>
+      <c r="O24" s="78"/>
+      <c r="P24" s="80">
+        <v>245</v>
+      </c>
+      <c r="Q24" s="78"/>
+      <c r="R24" s="78"/>
+      <c r="S24" s="78"/>
+      <c r="T24" s="78"/>
+      <c r="U24" s="78"/>
+      <c r="V24" s="78"/>
+      <c r="W24" s="78"/>
+      <c r="X24" s="78"/>
+      <c r="Y24" s="78"/>
+      <c r="Z24" s="78"/>
+      <c r="AA24" s="78"/>
+      <c r="AB24" s="78"/>
+      <c r="AC24" s="78"/>
+      <c r="AD24" s="78"/>
+    </row>
+    <row r="25" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="75">
+        <v>23</v>
+      </c>
+      <c r="B25" s="78"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="80">
+        <v>246</v>
+      </c>
+      <c r="F25" s="80">
+        <v>247</v>
+      </c>
+      <c r="G25" s="80">
+        <v>248</v>
+      </c>
+      <c r="H25" s="80">
+        <v>249</v>
+      </c>
+      <c r="I25" s="80">
+        <v>250</v>
+      </c>
+      <c r="J25" s="80">
+        <v>251</v>
+      </c>
+      <c r="K25" s="80">
+        <v>252</v>
+      </c>
+      <c r="L25" s="78"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="78"/>
+      <c r="O25" s="78"/>
+      <c r="P25" s="80">
+        <v>254</v>
+      </c>
+      <c r="Q25" s="78"/>
+      <c r="R25" s="78"/>
+      <c r="S25" s="78"/>
+      <c r="T25" s="78"/>
+      <c r="U25" s="78"/>
+      <c r="V25" s="78"/>
+      <c r="W25" s="78"/>
+      <c r="X25" s="78"/>
+      <c r="Y25" s="78"/>
+      <c r="Z25" s="78"/>
+      <c r="AA25" s="78"/>
+      <c r="AB25" s="78"/>
+      <c r="AC25" s="78"/>
+      <c r="AD25" s="78"/>
+    </row>
+    <row r="26" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="75">
+        <v>24</v>
+      </c>
+      <c r="B26" s="78"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="78"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="78"/>
+      <c r="G26" s="80">
+        <v>255</v>
+      </c>
+      <c r="H26" s="80">
+        <v>256</v>
+      </c>
+      <c r="I26" s="80">
+        <v>257</v>
+      </c>
+      <c r="J26" s="80">
+        <v>258</v>
+      </c>
+      <c r="K26" s="80">
+        <v>259</v>
+      </c>
+      <c r="L26" s="78"/>
+      <c r="M26" s="78"/>
+      <c r="N26" s="82" t="s">
+        <v>150</v>
+      </c>
+      <c r="O26" s="80">
+        <v>261</v>
+      </c>
+      <c r="P26" s="80">
+        <v>262</v>
+      </c>
+      <c r="Q26" s="78"/>
+      <c r="R26" s="78"/>
+      <c r="S26" s="78"/>
+      <c r="T26" s="78"/>
+      <c r="U26" s="78"/>
+      <c r="V26" s="78"/>
+      <c r="W26" s="78"/>
+      <c r="X26" s="78"/>
+      <c r="Y26" s="78"/>
+      <c r="Z26" s="78"/>
+      <c r="AA26" s="78"/>
+      <c r="AB26" s="78"/>
+      <c r="AC26" s="78"/>
+      <c r="AD26" s="78"/>
+    </row>
+    <row r="27" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="75">
+        <v>25</v>
+      </c>
+      <c r="B27" s="78"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="78"/>
+      <c r="F27" s="78"/>
+      <c r="G27" s="86">
+        <v>263</v>
+      </c>
+      <c r="H27" s="80">
+        <v>264</v>
+      </c>
+      <c r="I27" s="80">
+        <v>265</v>
+      </c>
+      <c r="J27" s="80">
+        <v>266</v>
+      </c>
+      <c r="K27" s="80">
+        <v>267</v>
+      </c>
+      <c r="L27" s="78"/>
+      <c r="M27" s="78"/>
+      <c r="N27" s="80">
+        <v>269</v>
+      </c>
+      <c r="O27" s="78"/>
+      <c r="P27" s="78"/>
+      <c r="Q27" s="78"/>
+      <c r="R27" s="78"/>
+      <c r="S27" s="78"/>
+      <c r="T27" s="78"/>
+      <c r="U27" s="78"/>
+      <c r="V27" s="78"/>
+      <c r="W27" s="78"/>
+      <c r="X27" s="78"/>
+      <c r="Y27" s="78"/>
+      <c r="Z27" s="78"/>
+      <c r="AA27" s="78"/>
+      <c r="AB27" s="78"/>
+      <c r="AC27" s="78"/>
+      <c r="AD27" s="78"/>
+    </row>
+    <row r="28" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="75">
+        <v>26</v>
+      </c>
+      <c r="B28" s="78"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="78"/>
+      <c r="F28" s="78"/>
+      <c r="G28" s="80">
+        <v>270</v>
+      </c>
+      <c r="H28" s="80">
+        <v>271</v>
+      </c>
+      <c r="I28" s="80">
+        <v>272</v>
+      </c>
+      <c r="J28" s="78"/>
+      <c r="K28" s="78"/>
+      <c r="L28" s="78"/>
+      <c r="M28" s="82" t="s">
+        <v>149</v>
+      </c>
+      <c r="N28" s="80">
+        <v>274</v>
+      </c>
+      <c r="O28" s="78"/>
+      <c r="P28" s="78"/>
+      <c r="Q28" s="78"/>
+      <c r="R28" s="78"/>
+      <c r="S28" s="78"/>
+      <c r="T28" s="78"/>
+      <c r="U28" s="78"/>
+      <c r="V28" s="78"/>
+      <c r="W28" s="78"/>
+      <c r="X28" s="78"/>
+      <c r="Y28" s="78"/>
+      <c r="Z28" s="78"/>
+      <c r="AA28" s="78"/>
+      <c r="AB28" s="78"/>
+      <c r="AC28" s="78"/>
+      <c r="AD28" s="78"/>
+    </row>
+    <row r="29" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="75">
+        <v>27</v>
+      </c>
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="78"/>
+      <c r="F29" s="78"/>
+      <c r="G29" s="80">
+        <v>275</v>
+      </c>
+      <c r="H29" s="80">
+        <v>276</v>
+      </c>
+      <c r="I29" s="80">
+        <v>277</v>
+      </c>
+      <c r="J29" s="78"/>
+      <c r="K29" s="78"/>
+      <c r="L29" s="80">
+        <v>278</v>
+      </c>
+      <c r="M29" s="80">
+        <v>279</v>
+      </c>
+      <c r="N29" s="80">
+        <v>280</v>
+      </c>
+      <c r="O29" s="80">
+        <v>281</v>
+      </c>
+      <c r="P29" s="80">
+        <v>282</v>
+      </c>
+      <c r="Q29" s="80">
+        <v>283</v>
+      </c>
+      <c r="R29" s="80">
+        <v>284</v>
+      </c>
+      <c r="S29" s="80">
+        <v>285</v>
+      </c>
+      <c r="T29" s="78"/>
+      <c r="U29" s="78"/>
+      <c r="V29" s="78"/>
+      <c r="W29" s="78"/>
+      <c r="X29" s="78"/>
+      <c r="Y29" s="78"/>
+      <c r="Z29" s="78"/>
+      <c r="AA29" s="78"/>
+      <c r="AB29" s="78"/>
+      <c r="AC29" s="78"/>
+      <c r="AD29" s="78"/>
+    </row>
+    <row r="30" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="75">
+        <v>28</v>
+      </c>
+      <c r="B30" s="78"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="80">
+        <v>286</v>
+      </c>
+      <c r="I30" s="80">
+        <v>287</v>
+      </c>
+      <c r="J30" s="78"/>
+      <c r="K30" s="78"/>
+      <c r="L30" s="78"/>
+      <c r="M30" s="78"/>
+      <c r="N30" s="78"/>
+      <c r="O30" s="78"/>
+      <c r="P30" s="78"/>
+      <c r="Q30" s="78"/>
+      <c r="R30" s="80">
+        <v>288</v>
+      </c>
+      <c r="S30" s="81">
+        <v>289</v>
+      </c>
+      <c r="T30" s="78"/>
+      <c r="U30" s="78"/>
+      <c r="V30" s="78"/>
+      <c r="W30" s="78"/>
+      <c r="X30" s="78"/>
+      <c r="Y30" s="78"/>
+      <c r="Z30" s="78"/>
+      <c r="AA30" s="78"/>
+      <c r="AB30" s="78"/>
+      <c r="AC30" s="78"/>
+      <c r="AD30" s="78"/>
+    </row>
+    <row r="31" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="75">
+        <v>29</v>
+      </c>
+      <c r="B31" s="78"/>
+      <c r="C31" s="78"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="78"/>
+      <c r="F31" s="78"/>
+      <c r="G31" s="78"/>
+      <c r="H31" s="80">
+        <v>290</v>
+      </c>
+      <c r="I31" s="78"/>
+      <c r="J31" s="78"/>
+      <c r="K31" s="78"/>
+      <c r="L31" s="78"/>
+      <c r="M31" s="78"/>
+      <c r="N31" s="78"/>
+      <c r="O31" s="78"/>
+      <c r="P31" s="78"/>
+      <c r="Q31" s="78"/>
+      <c r="R31" s="78"/>
+      <c r="S31" s="78"/>
+      <c r="T31" s="78"/>
+      <c r="U31" s="78"/>
+      <c r="V31" s="78"/>
+      <c r="W31" s="78"/>
+      <c r="X31" s="78"/>
+      <c r="Y31" s="78"/>
+      <c r="Z31" s="78"/>
+      <c r="AA31" s="78"/>
+      <c r="AB31" s="78"/>
+      <c r="AC31" s="78"/>
+      <c r="AD31" s="78"/>
+    </row>
+    <row r="32" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="75">
+        <v>30</v>
+      </c>
+      <c r="B32" s="78"/>
+      <c r="C32" s="78"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="78"/>
+      <c r="F32" s="78"/>
+      <c r="G32" s="78"/>
+      <c r="H32" s="80">
+        <v>291</v>
+      </c>
+      <c r="I32" s="78"/>
+      <c r="J32" s="78"/>
+      <c r="K32" s="78"/>
+      <c r="L32" s="78"/>
+      <c r="M32" s="78"/>
+      <c r="N32" s="78"/>
+      <c r="O32" s="78"/>
+      <c r="P32" s="78"/>
+      <c r="Q32" s="78"/>
+      <c r="R32" s="78"/>
+      <c r="S32" s="78"/>
+      <c r="T32" s="78"/>
+      <c r="U32" s="78"/>
+      <c r="V32" s="78"/>
+      <c r="W32" s="78"/>
+      <c r="X32" s="78"/>
+      <c r="Y32" s="78"/>
+      <c r="Z32" s="78"/>
+      <c r="AA32" s="78"/>
+      <c r="AB32" s="78"/>
+      <c r="AC32" s="78"/>
+      <c r="AD32" s="78"/>
+    </row>
+    <row r="33" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="75">
+        <v>31</v>
+      </c>
+      <c r="B33" s="78"/>
+      <c r="C33" s="78"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="78"/>
+      <c r="H33" s="81" t="s">
+        <v>185</v>
+      </c>
+      <c r="I33" s="78"/>
+      <c r="J33" s="78"/>
+      <c r="K33" s="78"/>
+      <c r="L33" s="78"/>
+      <c r="M33" s="78"/>
+      <c r="N33" s="78"/>
+      <c r="O33" s="78"/>
+      <c r="P33" s="78"/>
+      <c r="Q33" s="78"/>
+      <c r="R33" s="78"/>
+      <c r="S33" s="78"/>
+      <c r="T33" s="78"/>
+      <c r="U33" s="78"/>
+      <c r="V33" s="78"/>
+      <c r="W33" s="78"/>
+      <c r="X33" s="78"/>
+      <c r="Y33" s="78"/>
+      <c r="Z33" s="78"/>
+      <c r="AA33" s="78"/>
+      <c r="AB33" s="78"/>
+      <c r="AC33" s="78"/>
+      <c r="AD33" s="78"/>
+    </row>
+    <row r="34" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="76"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="46"/>
+      <c r="M34" s="46"/>
+      <c r="N34" s="46"/>
+      <c r="O34" s="46"/>
+      <c r="P34" s="46"/>
+      <c r="Q34" s="46"/>
+      <c r="R34" s="46"/>
+      <c r="S34" s="46"/>
+      <c r="T34" s="46"/>
+      <c r="U34" s="46"/>
+      <c r="V34" s="46"/>
+      <c r="W34" s="46"/>
+      <c r="X34" s="46"/>
+      <c r="Y34" s="46"/>
+      <c r="Z34" s="46"/>
+      <c r="AA34" s="46"/>
+      <c r="AB34" s="46"/>
+      <c r="AC34" s="46"/>
+      <c r="AD34" s="46"/>
+    </row>
+    <row r="35" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="76"/>
+      <c r="B35" s="46"/>
+      <c r="C35" s="46"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="46"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="46"/>
+      <c r="O35" s="46"/>
+      <c r="P35" s="46"/>
+      <c r="Q35" s="46"/>
+      <c r="R35" s="46"/>
+      <c r="S35" s="46"/>
+      <c r="T35" s="46"/>
+      <c r="U35" s="46"/>
+      <c r="V35" s="46"/>
+      <c r="W35" s="46"/>
+      <c r="X35" s="46"/>
+      <c r="Y35" s="46"/>
+      <c r="Z35" s="46"/>
+      <c r="AA35" s="46"/>
+      <c r="AB35" s="46"/>
+      <c r="AC35" s="46"/>
+      <c r="AD35" s="46"/>
+    </row>
+    <row r="36" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="76"/>
+      <c r="B36" s="46"/>
+      <c r="C36" s="46"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="46"/>
+      <c r="N36" s="49"/>
+      <c r="O36" s="46"/>
+      <c r="P36" s="46"/>
+      <c r="Q36" s="46"/>
+      <c r="R36" s="46"/>
+      <c r="S36" s="46"/>
+      <c r="T36" s="46"/>
+      <c r="U36" s="46"/>
+      <c r="V36" s="46"/>
+      <c r="W36" s="46"/>
+      <c r="X36" s="46"/>
+      <c r="Y36" s="46"/>
+      <c r="Z36" s="46"/>
+      <c r="AA36" s="46"/>
+      <c r="AB36" s="46"/>
+      <c r="AC36" s="46"/>
+      <c r="AD36" s="46"/>
+    </row>
+    <row r="37" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="76"/>
+      <c r="B37" s="46"/>
+      <c r="C37" s="46"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
+      <c r="J37" s="46"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="46"/>
+      <c r="M37" s="46"/>
+      <c r="N37" s="46"/>
+      <c r="O37" s="46"/>
+      <c r="P37" s="46"/>
+      <c r="Q37" s="46"/>
+      <c r="R37" s="46"/>
+      <c r="S37" s="46"/>
+      <c r="T37" s="46"/>
+      <c r="U37" s="46"/>
+      <c r="V37" s="46"/>
+      <c r="W37" s="46"/>
+      <c r="X37" s="46"/>
+      <c r="Y37" s="46"/>
+      <c r="Z37" s="46"/>
+      <c r="AA37" s="46"/>
+      <c r="AB37" s="46"/>
+      <c r="AC37" s="46"/>
+      <c r="AD37" s="46"/>
+    </row>
+    <row r="38" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="76"/>
+      <c r="B38" s="46"/>
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
+      <c r="J38" s="46"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="46"/>
+      <c r="M38" s="46"/>
+      <c r="N38" s="46"/>
+      <c r="O38" s="46"/>
+      <c r="P38" s="46"/>
+      <c r="Q38" s="46"/>
+      <c r="R38" s="46"/>
+      <c r="S38" s="46"/>
+      <c r="T38" s="46"/>
+      <c r="U38" s="46"/>
+      <c r="V38" s="46"/>
+      <c r="W38" s="46"/>
+      <c r="X38" s="46"/>
+      <c r="Y38" s="46"/>
+      <c r="Z38" s="46"/>
+      <c r="AA38" s="46"/>
+      <c r="AB38" s="46"/>
+      <c r="AC38" s="46"/>
+      <c r="AD38" s="46"/>
+    </row>
+    <row r="39" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="76"/>
+      <c r="B39" s="46"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="46"/>
+      <c r="M39" s="46"/>
+      <c r="N39" s="46"/>
+      <c r="O39" s="46"/>
+      <c r="P39" s="46"/>
+      <c r="AD39" s="46"/>
+    </row>
+    <row r="40" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="76"/>
+      <c r="B40" s="49"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="46"/>
+      <c r="M40" s="46"/>
+      <c r="N40" s="46"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="49"/>
+      <c r="AD40" s="49"/>
+    </row>
+    <row r="41" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="76"/>
+      <c r="B41" s="49"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="49"/>
+      <c r="O41" s="49"/>
+      <c r="P41" s="49"/>
+      <c r="AD41" s="49"/>
+    </row>
+    <row r="42" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="76"/>
+      <c r="B42" s="49"/>
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49"/>
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="AD42" s="49"/>
+    </row>
+    <row r="43" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="76"/>
+      <c r="B43" s="49"/>
+      <c r="K43" s="49"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="49"/>
+      <c r="O43" s="49"/>
+      <c r="P43" s="49"/>
+      <c r="AD43" s="49"/>
+    </row>
+    <row r="44" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="76"/>
+      <c r="B44" s="49"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="49"/>
+      <c r="O44" s="49"/>
+      <c r="P44" s="49"/>
+      <c r="AD44" s="49"/>
+    </row>
+    <row r="45" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="76"/>
+      <c r="B45" s="49"/>
+      <c r="K45" s="49"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="49"/>
+      <c r="O45" s="49"/>
+      <c r="P45" s="49"/>
+      <c r="AD45" s="49"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="U7" twoDigitTextYear="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0919FBA-A3A9-4ADF-8571-ADEF5FC84896}">
   <dimension ref="A1:AM37"/>
   <sheetViews>
@@ -11851,12 +13947,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B972C991-F8C9-4FE0-9BA0-7BB309CE3C64}">
   <dimension ref="A1:AU55"/>
   <sheetViews>
     <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+      <selection activeCell="AD57" sqref="AD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14873,11 +16969,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B7C2B5-A3F4-4A6B-913D-2117547F5F2B}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
@@ -14892,45 +16988,45 @@
   <sheetData>
     <row r="1" spans="1:12" s="72" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="73" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" s="73" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C1" s="73" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D1" s="74" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E1" s="74" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F1" s="73" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G1" s="73" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H1" s="72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I1" s="72" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J1" s="72" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K1" s="72" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L1" s="72" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2" s="40">
         <v>7</v>
@@ -14953,16 +17049,16 @@
         <v>200</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L2" s="4" t="str">
         <f>_xlfn.CONCAT(H2,B1,J2,B2,I2,C1,J2,C2,I2,F1,J2,F2,I2,G1,J2,G2,K2,I2)</f>
@@ -14971,7 +17067,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="70" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B4" s="40">
         <v>384</v>
@@ -14979,7 +17075,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="70" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B5" s="40">
         <v>240</v>
@@ -14987,30 +17083,30 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="73" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="73" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="73" t="s">
         <v>179</v>
       </c>
-      <c r="B7" s="73" t="s">
-        <v>182</v>
-      </c>
-      <c r="C7" s="73" t="s">
+      <c r="E7" s="73" t="s">
+        <v>180</v>
+      </c>
+      <c r="F7" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="74" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="87" t="s">
         <v>183</v>
-      </c>
-      <c r="D7" s="73" t="s">
-        <v>180</v>
-      </c>
-      <c r="E7" s="73" t="s">
-        <v>181</v>
-      </c>
-      <c r="F7" s="74" t="s">
-        <v>175</v>
-      </c>
-      <c r="G7" s="74" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="75" t="s">
-        <v>184</v>
       </c>
       <c r="B8" s="40">
         <v>132</v>
@@ -15038,7 +17134,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="76"/>
+      <c r="A9" s="88"/>
       <c r="B9" s="40">
         <v>28</v>
       </c>
@@ -15065,7 +17161,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="76"/>
+      <c r="A10" s="88"/>
       <c r="B10" s="40">
         <v>132</v>
       </c>
@@ -15092,7 +17188,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="76"/>
+      <c r="A11" s="88"/>
       <c r="B11" s="40">
         <v>216</v>
       </c>
@@ -15119,7 +17215,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="76"/>
+      <c r="A12" s="88"/>
       <c r="B12" s="40">
         <v>132</v>
       </c>
@@ -15146,7 +17242,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="76"/>
+      <c r="A13" s="88"/>
       <c r="B13" s="40">
         <v>228</v>
       </c>
@@ -15173,7 +17269,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="76"/>
+      <c r="A14" s="88"/>
       <c r="B14" s="40">
         <v>40</v>
       </c>
@@ -15200,7 +17296,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="76"/>
+      <c r="A15" s="88"/>
       <c r="B15" s="40">
         <v>132</v>
       </c>

</xml_diff>

<commit_message>
Forest of Torian map data done and imported, but...
I haven't implemented the fairy fountain animation and translated all the signs of the Forest of Torian yet.
</commit_message>
<xml_diff>
--- a/Planning/OverworldMap.xlsx
+++ b/Planning/OverworldMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\Repos\ZeldasAdventureRemastered\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606D60D2-BC21-4F17-871A-5647F75297A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB4A599-B12F-47A2-B1A8-14BABA5BF52C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{2A32EC26-D8CF-452B-B3E7-5B8DBE295FDC}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="7" xr2:uid="{2A32EC26-D8CF-452B-B3E7-5B8DBE295FDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Music" sheetId="1" r:id="rId1"/>
@@ -1574,7 +1574,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K14" sqref="K14"/>
+      <selection pane="topRight" activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10570,7 +10570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8A283EA-E136-4164-BE4B-388B47B94988}">
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="V15" sqref="V15"/>
     </sheetView>
@@ -16973,8 +16973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B7C2B5-A3F4-4A6B-913D-2117547F5F2B}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17029,24 +17029,24 @@
         <v>184</v>
       </c>
       <c r="B2" s="40">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C2" s="40">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="71">
-        <v>2892</v>
+        <v>6412</v>
       </c>
       <c r="E2" s="71">
-        <v>2840</v>
+        <v>2460</v>
       </c>
       <c r="F2" s="40">
         <f>SUM(D2-B2*$B$4)</f>
-        <v>204</v>
+        <v>268</v>
       </c>
       <c r="G2" s="40">
         <f>SUM(E2-C2*$B$5)</f>
-        <v>200</v>
+        <v>60</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>165</v>
@@ -17062,7 +17062,7 @@
       </c>
       <c r="L2" s="4" t="str">
         <f>_xlfn.CONCAT(H2,B1,J2,B2,I2,C1,J2,C2,I2,F1,J2,F2,I2,G1,J2,G2,K2,I2)</f>
-        <v>{TileX:7,TileY:11,PlayerX:204,PlayerY:200},</v>
+        <v>{TileX:16,TileY:10,PlayerX:268,PlayerY:60},</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>